<commit_message>
Cleaning inbound referral data
</commit_message>
<xml_diff>
--- a/prepare_contacts/data/List of Contacts - Referrals - Inbound.xlsx
+++ b/prepare_contacts/data/List of Contacts - Referrals - Inbound.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29029"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BenjaminMcCarty\Documents\Git Repositories\JLG\JLG_Provider_Recommender\prepare_contacts\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1BECA7F-A1EA-4BDD-B9AD-40F73C52D2F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="List of Contacts - Referral..." sheetId="1" r:id="rId1"/>
@@ -14,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="557">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2687" uniqueCount="557">
   <si>
     <t>Project ID</t>
   </si>
@@ -1690,22 +1696,22 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="m/d/yyyy h:mm AM/PM"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="m/d/yyyy\ h:mm\ AM/PM"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
-      <color rgb="FFFFFFFF"/>
-      <sz val="11"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1736,32 +1742,36 @@
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="true" applyFill="true" applyAlignment="true">
-      <alignment wrapText="true"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="true" applyFill="true" applyAlignment="true">
-      <alignment horizontal="right" wrapText="true"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyAlignment="true">
-      <alignment wrapText="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyAlignment="true">
-      <alignment wrapText="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="27" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyAlignment="true">
-      <alignment wrapText="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyAlignment="true">
-      <alignment horizontal="right" wrapText="true"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -2063,15 +2073,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main">
-  <sheetPr/>
-  <dimension ref="A1:W537"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:V537"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" topLeftCell="A1" zoomScaleNormal="100" zoomScaleSheetLayoutView="60" zoomScale="100" view="normal"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" defaultColWidth="30"/>
+  <sheetFormatPr defaultColWidth="30" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" ht="28.25">
+    <row r="1" spans="1:22" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2139,7 +2148,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" ht="14.8">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A2" s="3">
         <v>991271227</v>
       </c>
@@ -2183,7 +2192,7 @@
       <c r="U2" s="6"/>
       <c r="V2" s="6"/>
     </row>
-    <row r="3" ht="28.25">
+    <row r="3" spans="1:22" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="3">
         <v>991272012</v>
       </c>
@@ -2227,7 +2236,7 @@
       <c r="U3" s="6"/>
       <c r="V3" s="6"/>
     </row>
-    <row r="4" ht="14.8">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A4" s="3">
         <v>991272170</v>
       </c>
@@ -2273,7 +2282,7 @@
       <c r="U4" s="6"/>
       <c r="V4" s="6"/>
     </row>
-    <row r="5" ht="14.8">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A5" s="3">
         <v>991272394</v>
       </c>
@@ -2319,7 +2328,7 @@
       <c r="U5" s="6"/>
       <c r="V5" s="6"/>
     </row>
-    <row r="6" ht="14.8">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A6" s="3">
         <v>991272748</v>
       </c>
@@ -2365,7 +2374,7 @@
       <c r="U6" s="6"/>
       <c r="V6" s="6"/>
     </row>
-    <row r="7" ht="14.8">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A7" s="3">
         <v>991272749</v>
       </c>
@@ -2413,7 +2422,7 @@
       <c r="U7" s="6"/>
       <c r="V7" s="6"/>
     </row>
-    <row r="8" ht="14.8">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A8" s="3">
         <v>991272763</v>
       </c>
@@ -2457,7 +2466,7 @@
       <c r="U8" s="6"/>
       <c r="V8" s="6"/>
     </row>
-    <row r="9" ht="14.8">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A9" s="3">
         <v>991272878</v>
       </c>
@@ -2503,7 +2512,7 @@
       <c r="U9" s="6"/>
       <c r="V9" s="6"/>
     </row>
-    <row r="10" ht="14.8">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A10" s="3">
         <v>991273056</v>
       </c>
@@ -2549,7 +2558,7 @@
       <c r="U10" s="6"/>
       <c r="V10" s="6"/>
     </row>
-    <row r="11" ht="14.8">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A11" s="3">
         <v>991273068</v>
       </c>
@@ -2597,7 +2606,7 @@
       <c r="U11" s="6"/>
       <c r="V11" s="6"/>
     </row>
-    <row r="12" ht="14.8">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A12" s="3">
         <v>991273109</v>
       </c>
@@ -2641,7 +2650,7 @@
       <c r="U12" s="6"/>
       <c r="V12" s="6"/>
     </row>
-    <row r="13" ht="14.8">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A13" s="3">
         <v>991273257</v>
       </c>
@@ -2689,7 +2698,7 @@
       <c r="U13" s="6"/>
       <c r="V13" s="6"/>
     </row>
-    <row r="14" ht="14.8">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A14" s="3">
         <v>991273382</v>
       </c>
@@ -2735,7 +2744,7 @@
       <c r="U14" s="6"/>
       <c r="V14" s="6"/>
     </row>
-    <row r="15" ht="14.8">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A15" s="3">
         <v>991273798</v>
       </c>
@@ -2781,7 +2790,7 @@
       <c r="U15" s="6"/>
       <c r="V15" s="6"/>
     </row>
-    <row r="16" ht="14.8">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A16" s="3">
         <v>991273836</v>
       </c>
@@ -2827,7 +2836,7 @@
       <c r="U16" s="6"/>
       <c r="V16" s="6"/>
     </row>
-    <row r="17" ht="14.8">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A17" s="3">
         <v>991274165</v>
       </c>
@@ -2867,7 +2876,7 @@
       <c r="U17" s="6"/>
       <c r="V17" s="6"/>
     </row>
-    <row r="18" ht="14.8">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A18" s="3">
         <v>991274589</v>
       </c>
@@ -2913,7 +2922,7 @@
       <c r="U18" s="6"/>
       <c r="V18" s="6"/>
     </row>
-    <row r="19" ht="14.8">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A19" s="3">
         <v>991274813</v>
       </c>
@@ -2951,7 +2960,7 @@
       <c r="U19" s="6"/>
       <c r="V19" s="6"/>
     </row>
-    <row r="20" ht="14.8">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A20" s="3">
         <v>991275049</v>
       </c>
@@ -2999,7 +3008,7 @@
       <c r="U20" s="6"/>
       <c r="V20" s="6"/>
     </row>
-    <row r="21" ht="28.25">
+    <row r="21" spans="1:22" ht="29" x14ac:dyDescent="0.35">
       <c r="A21" s="3">
         <v>991275076</v>
       </c>
@@ -3043,7 +3052,7 @@
       <c r="U21" s="6"/>
       <c r="V21" s="6"/>
     </row>
-    <row r="22" ht="14.8">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A22" s="3">
         <v>991275195</v>
       </c>
@@ -3089,7 +3098,7 @@
       <c r="U22" s="6"/>
       <c r="V22" s="6"/>
     </row>
-    <row r="23" ht="14.8">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A23" s="3">
         <v>991275336</v>
       </c>
@@ -3135,7 +3144,7 @@
       <c r="U23" s="6"/>
       <c r="V23" s="6"/>
     </row>
-    <row r="24" ht="14.8">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A24" s="3">
         <v>991275402</v>
       </c>
@@ -3183,7 +3192,7 @@
       <c r="U24" s="6"/>
       <c r="V24" s="6"/>
     </row>
-    <row r="25" ht="28.25">
+    <row r="25" spans="1:22" ht="29" x14ac:dyDescent="0.35">
       <c r="A25" s="3">
         <v>991275617</v>
       </c>
@@ -3229,7 +3238,7 @@
       <c r="U25" s="6"/>
       <c r="V25" s="6"/>
     </row>
-    <row r="26" ht="14.8">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A26" s="3">
         <v>991275744</v>
       </c>
@@ -3275,7 +3284,7 @@
       <c r="U26" s="6"/>
       <c r="V26" s="6"/>
     </row>
-    <row r="27" ht="14.8">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A27" s="3">
         <v>991275800</v>
       </c>
@@ -3319,7 +3328,7 @@
       <c r="U27" s="6"/>
       <c r="V27" s="6"/>
     </row>
-    <row r="28" ht="14.8">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A28" s="3">
         <v>991275996</v>
       </c>
@@ -3365,7 +3374,7 @@
       <c r="U28" s="6"/>
       <c r="V28" s="6"/>
     </row>
-    <row r="29" ht="14.8">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A29" s="3">
         <v>991276109</v>
       </c>
@@ -3411,7 +3420,7 @@
       <c r="U29" s="6"/>
       <c r="V29" s="6"/>
     </row>
-    <row r="30" ht="28.25">
+    <row r="30" spans="1:22" ht="29" x14ac:dyDescent="0.35">
       <c r="A30" s="3">
         <v>991276270</v>
       </c>
@@ -3469,7 +3478,7 @@
       <c r="U30" s="6"/>
       <c r="V30" s="6"/>
     </row>
-    <row r="31" ht="14.8">
+    <row r="31" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A31" s="3">
         <v>991276389</v>
       </c>
@@ -3515,7 +3524,7 @@
       <c r="U31" s="6"/>
       <c r="V31" s="6"/>
     </row>
-    <row r="32" ht="14.8">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A32" s="3">
         <v>991276578</v>
       </c>
@@ -3561,7 +3570,7 @@
       <c r="U32" s="6"/>
       <c r="V32" s="6"/>
     </row>
-    <row r="33" ht="28.25">
+    <row r="33" spans="1:22" ht="29" x14ac:dyDescent="0.35">
       <c r="A33" s="3">
         <v>991276984</v>
       </c>
@@ -3605,7 +3614,7 @@
       <c r="U33" s="6"/>
       <c r="V33" s="6"/>
     </row>
-    <row r="34" ht="14.8">
+    <row r="34" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A34" s="3">
         <v>991276996</v>
       </c>
@@ -3649,7 +3658,7 @@
       <c r="U34" s="6"/>
       <c r="V34" s="6"/>
     </row>
-    <row r="35" ht="14.8">
+    <row r="35" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A35" s="3">
         <v>991277144</v>
       </c>
@@ -3695,7 +3704,7 @@
       <c r="U35" s="6"/>
       <c r="V35" s="6"/>
     </row>
-    <row r="36" ht="14.8">
+    <row r="36" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A36" s="3">
         <v>991277607</v>
       </c>
@@ -3745,7 +3754,7 @@
       <c r="U36" s="6"/>
       <c r="V36" s="6"/>
     </row>
-    <row r="37" ht="14.8">
+    <row r="37" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A37" s="3">
         <v>991277752</v>
       </c>
@@ -3791,7 +3800,7 @@
       <c r="U37" s="6"/>
       <c r="V37" s="6"/>
     </row>
-    <row r="38" ht="14.8">
+    <row r="38" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A38" s="3">
         <v>991277786</v>
       </c>
@@ -3839,7 +3848,7 @@
       <c r="U38" s="6"/>
       <c r="V38" s="6"/>
     </row>
-    <row r="39" ht="14.8">
+    <row r="39" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A39" s="3">
         <v>991278021</v>
       </c>
@@ -3885,7 +3894,7 @@
       <c r="U39" s="6"/>
       <c r="V39" s="6"/>
     </row>
-    <row r="40" ht="14.8">
+    <row r="40" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A40" s="3">
         <v>991278027</v>
       </c>
@@ -3933,7 +3942,7 @@
       <c r="U40" s="6"/>
       <c r="V40" s="6"/>
     </row>
-    <row r="41" ht="14.8">
+    <row r="41" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A41" s="3">
         <v>991278768</v>
       </c>
@@ -3979,7 +3988,7 @@
       <c r="U41" s="6"/>
       <c r="V41" s="6"/>
     </row>
-    <row r="42" ht="14.8">
+    <row r="42" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A42" s="3">
         <v>991279395</v>
       </c>
@@ -4025,7 +4034,7 @@
       <c r="U42" s="6"/>
       <c r="V42" s="6"/>
     </row>
-    <row r="43" ht="14.8">
+    <row r="43" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A43" s="3">
         <v>991279559</v>
       </c>
@@ -4073,7 +4082,7 @@
       <c r="U43" s="6"/>
       <c r="V43" s="6"/>
     </row>
-    <row r="44" ht="14.8">
+    <row r="44" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A44" s="3">
         <v>991280147</v>
       </c>
@@ -4117,7 +4126,7 @@
       <c r="U44" s="6"/>
       <c r="V44" s="6"/>
     </row>
-    <row r="45" ht="14.8">
+    <row r="45" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A45" s="3">
         <v>991280237</v>
       </c>
@@ -4163,7 +4172,7 @@
       <c r="U45" s="6"/>
       <c r="V45" s="6"/>
     </row>
-    <row r="46" ht="14.8">
+    <row r="46" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A46" s="3">
         <v>991280263</v>
       </c>
@@ -4209,7 +4218,7 @@
       <c r="U46" s="6"/>
       <c r="V46" s="6"/>
     </row>
-    <row r="47" ht="14.8">
+    <row r="47" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A47" s="3">
         <v>991280312</v>
       </c>
@@ -4257,7 +4266,7 @@
       <c r="U47" s="6"/>
       <c r="V47" s="6"/>
     </row>
-    <row r="48" ht="14.8">
+    <row r="48" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A48" s="3">
         <v>991280947</v>
       </c>
@@ -4305,7 +4314,7 @@
       <c r="U48" s="6"/>
       <c r="V48" s="6"/>
     </row>
-    <row r="49" ht="14.8">
+    <row r="49" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A49" s="3">
         <v>991281165</v>
       </c>
@@ -4353,7 +4362,7 @@
       <c r="U49" s="6"/>
       <c r="V49" s="6"/>
     </row>
-    <row r="50" ht="28.25">
+    <row r="50" spans="1:22" ht="29" x14ac:dyDescent="0.35">
       <c r="A50" s="3">
         <v>991281240</v>
       </c>
@@ -4397,7 +4406,7 @@
       <c r="U50" s="6"/>
       <c r="V50" s="6"/>
     </row>
-    <row r="51" ht="14.8">
+    <row r="51" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A51" s="3">
         <v>991281388</v>
       </c>
@@ -4445,7 +4454,7 @@
       <c r="U51" s="6"/>
       <c r="V51" s="6"/>
     </row>
-    <row r="52" ht="14.8">
+    <row r="52" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A52" s="3">
         <v>991281643</v>
       </c>
@@ -4491,7 +4500,7 @@
       <c r="U52" s="6"/>
       <c r="V52" s="6"/>
     </row>
-    <row r="53" ht="14.8">
+    <row r="53" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A53" s="3">
         <v>991281725</v>
       </c>
@@ -4539,7 +4548,7 @@
       <c r="U53" s="6"/>
       <c r="V53" s="6"/>
     </row>
-    <row r="54" ht="14.8">
+    <row r="54" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A54" s="3">
         <v>991281727</v>
       </c>
@@ -4587,7 +4596,7 @@
       <c r="U54" s="6"/>
       <c r="V54" s="6"/>
     </row>
-    <row r="55" ht="14.8">
+    <row r="55" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A55" s="3">
         <v>991318272</v>
       </c>
@@ -4635,7 +4644,7 @@
       <c r="U55" s="6"/>
       <c r="V55" s="6"/>
     </row>
-    <row r="56" ht="14.8">
+    <row r="56" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A56" s="3">
         <v>991318720</v>
       </c>
@@ -4683,7 +4692,7 @@
       <c r="U56" s="6"/>
       <c r="V56" s="6"/>
     </row>
-    <row r="57" ht="14.8">
+    <row r="57" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A57" s="3">
         <v>991318741</v>
       </c>
@@ -4731,7 +4740,7 @@
       <c r="U57" s="6"/>
       <c r="V57" s="6"/>
     </row>
-    <row r="58" ht="14.8">
+    <row r="58" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A58" s="3">
         <v>991348724</v>
       </c>
@@ -4779,7 +4788,7 @@
       <c r="U58" s="6"/>
       <c r="V58" s="6"/>
     </row>
-    <row r="59" ht="14.8">
+    <row r="59" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A59" s="3">
         <v>991349016</v>
       </c>
@@ -4827,7 +4836,7 @@
       <c r="U59" s="6"/>
       <c r="V59" s="6"/>
     </row>
-    <row r="60" ht="14.8">
+    <row r="60" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A60" s="3">
         <v>991349466</v>
       </c>
@@ -4875,7 +4884,7 @@
       <c r="U60" s="6"/>
       <c r="V60" s="6"/>
     </row>
-    <row r="61" ht="14.8">
+    <row r="61" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A61" s="3">
         <v>991349758</v>
       </c>
@@ -4923,7 +4932,7 @@
       <c r="U61" s="6"/>
       <c r="V61" s="6"/>
     </row>
-    <row r="62" ht="14.8">
+    <row r="62" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A62" s="3">
         <v>991349991</v>
       </c>
@@ -4971,7 +4980,7 @@
       <c r="U62" s="6"/>
       <c r="V62" s="6"/>
     </row>
-    <row r="63" ht="14.8">
+    <row r="63" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A63" s="3">
         <v>991350385</v>
       </c>
@@ -5019,7 +5028,7 @@
       <c r="U63" s="6"/>
       <c r="V63" s="6"/>
     </row>
-    <row r="64" ht="14.8">
+    <row r="64" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A64" s="3">
         <v>991350648</v>
       </c>
@@ -5067,7 +5076,7 @@
       <c r="U64" s="6"/>
       <c r="V64" s="6"/>
     </row>
-    <row r="65" ht="14.8">
+    <row r="65" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A65" s="3">
         <v>991350812</v>
       </c>
@@ -5115,7 +5124,7 @@
       <c r="U65" s="6"/>
       <c r="V65" s="6"/>
     </row>
-    <row r="66" ht="14.8">
+    <row r="66" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A66" s="3">
         <v>991350815</v>
       </c>
@@ -5163,7 +5172,7 @@
       <c r="U66" s="6"/>
       <c r="V66" s="6"/>
     </row>
-    <row r="67" ht="14.8">
+    <row r="67" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A67" s="3">
         <v>991350816</v>
       </c>
@@ -5211,7 +5220,7 @@
       <c r="U67" s="6"/>
       <c r="V67" s="6"/>
     </row>
-    <row r="68" ht="14.8">
+    <row r="68" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A68" s="3">
         <v>991350818</v>
       </c>
@@ -5259,7 +5268,7 @@
       <c r="U68" s="6"/>
       <c r="V68" s="6"/>
     </row>
-    <row r="69" ht="14.8">
+    <row r="69" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A69" s="3">
         <v>991350819</v>
       </c>
@@ -5305,7 +5314,7 @@
       <c r="U69" s="6"/>
       <c r="V69" s="6"/>
     </row>
-    <row r="70" ht="14.8">
+    <row r="70" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A70" s="3">
         <v>991350820</v>
       </c>
@@ -5351,7 +5360,7 @@
       <c r="U70" s="6"/>
       <c r="V70" s="6"/>
     </row>
-    <row r="71" ht="14.8">
+    <row r="71" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A71" s="3">
         <v>991350821</v>
       </c>
@@ -5399,7 +5408,7 @@
       <c r="U71" s="6"/>
       <c r="V71" s="6"/>
     </row>
-    <row r="72" ht="14.8">
+    <row r="72" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A72" s="3">
         <v>991352780</v>
       </c>
@@ -5443,7 +5452,7 @@
       <c r="U72" s="6"/>
       <c r="V72" s="6"/>
     </row>
-    <row r="73" ht="14.8">
+    <row r="73" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A73" s="3">
         <v>991353283</v>
       </c>
@@ -5491,7 +5500,7 @@
       <c r="U73" s="6"/>
       <c r="V73" s="6"/>
     </row>
-    <row r="74" ht="14.8">
+    <row r="74" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A74" s="3">
         <v>991353408</v>
       </c>
@@ -5539,7 +5548,7 @@
       <c r="U74" s="6"/>
       <c r="V74" s="6"/>
     </row>
-    <row r="75" ht="14.8">
+    <row r="75" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A75" s="3">
         <v>991353470</v>
       </c>
@@ -5587,7 +5596,7 @@
       <c r="U75" s="6"/>
       <c r="V75" s="6"/>
     </row>
-    <row r="76" ht="14.8">
+    <row r="76" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A76" s="3">
         <v>991353683</v>
       </c>
@@ -5635,7 +5644,7 @@
       <c r="U76" s="6"/>
       <c r="V76" s="6"/>
     </row>
-    <row r="77" ht="14.8">
+    <row r="77" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A77" s="3">
         <v>991353824</v>
       </c>
@@ -5675,7 +5684,7 @@
       <c r="U77" s="6"/>
       <c r="V77" s="6"/>
     </row>
-    <row r="78" ht="14.8">
+    <row r="78" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A78" s="3">
         <v>991353853</v>
       </c>
@@ -5715,7 +5724,7 @@
       <c r="U78" s="6"/>
       <c r="V78" s="6"/>
     </row>
-    <row r="79" ht="14.8">
+    <row r="79" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A79" s="3">
         <v>991353916</v>
       </c>
@@ -5763,7 +5772,7 @@
       <c r="U79" s="6"/>
       <c r="V79" s="6"/>
     </row>
-    <row r="80" ht="14.8">
+    <row r="80" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A80" s="3">
         <v>991354027</v>
       </c>
@@ -5811,7 +5820,7 @@
       <c r="U80" s="6"/>
       <c r="V80" s="6"/>
     </row>
-    <row r="81" ht="14.8">
+    <row r="81" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A81" s="3">
         <v>991355968</v>
       </c>
@@ -5859,7 +5868,7 @@
       <c r="U81" s="6"/>
       <c r="V81" s="6"/>
     </row>
-    <row r="82" ht="14.8">
+    <row r="82" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A82" s="3">
         <v>991357380</v>
       </c>
@@ -5907,7 +5916,7 @@
       <c r="U82" s="6"/>
       <c r="V82" s="6"/>
     </row>
-    <row r="83" ht="14.8">
+    <row r="83" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A83" s="3">
         <v>991357525</v>
       </c>
@@ -5959,7 +5968,7 @@
       <c r="U83" s="6"/>
       <c r="V83" s="6"/>
     </row>
-    <row r="84" ht="14.8">
+    <row r="84" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A84" s="3">
         <v>991359250</v>
       </c>
@@ -6019,7 +6028,7 @@
       <c r="U84" s="6"/>
       <c r="V84" s="6"/>
     </row>
-    <row r="85" ht="14.8">
+    <row r="85" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A85" s="3">
         <v>991359301</v>
       </c>
@@ -6079,7 +6088,7 @@
       <c r="U85" s="6"/>
       <c r="V85" s="6"/>
     </row>
-    <row r="86" ht="28.25">
+    <row r="86" spans="1:22" ht="29" x14ac:dyDescent="0.35">
       <c r="A86" s="3">
         <v>991360086</v>
       </c>
@@ -6127,7 +6136,7 @@
       <c r="U86" s="6"/>
       <c r="V86" s="6"/>
     </row>
-    <row r="87" ht="14.8">
+    <row r="87" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A87" s="3">
         <v>991360480</v>
       </c>
@@ -6175,7 +6184,7 @@
       <c r="U87" s="6"/>
       <c r="V87" s="6"/>
     </row>
-    <row r="88" ht="14.8">
+    <row r="88" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A88" s="3">
         <v>991360585</v>
       </c>
@@ -6223,7 +6232,7 @@
       <c r="U88" s="6"/>
       <c r="V88" s="6"/>
     </row>
-    <row r="89" ht="14.8">
+    <row r="89" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A89" s="3">
         <v>991360713</v>
       </c>
@@ -6271,7 +6280,7 @@
       <c r="U89" s="6"/>
       <c r="V89" s="6"/>
     </row>
-    <row r="90" ht="14.8">
+    <row r="90" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A90" s="3">
         <v>991360732</v>
       </c>
@@ -6319,7 +6328,7 @@
       <c r="U90" s="6"/>
       <c r="V90" s="6"/>
     </row>
-    <row r="91" ht="14.8">
+    <row r="91" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A91" s="3">
         <v>991362485</v>
       </c>
@@ -6359,7 +6368,7 @@
       <c r="U91" s="6"/>
       <c r="V91" s="6"/>
     </row>
-    <row r="92" ht="14.8">
+    <row r="92" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A92" s="3">
         <v>991362754</v>
       </c>
@@ -6407,7 +6416,7 @@
       <c r="U92" s="6"/>
       <c r="V92" s="6"/>
     </row>
-    <row r="93" ht="14.8">
+    <row r="93" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A93" s="3">
         <v>991362769</v>
       </c>
@@ -6455,7 +6464,7 @@
       <c r="U93" s="6"/>
       <c r="V93" s="6"/>
     </row>
-    <row r="94" ht="14.8">
+    <row r="94" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A94" s="3">
         <v>991362773</v>
       </c>
@@ -6503,7 +6512,7 @@
       <c r="U94" s="6"/>
       <c r="V94" s="6"/>
     </row>
-    <row r="95" ht="14.8">
+    <row r="95" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A95" s="3">
         <v>991365404</v>
       </c>
@@ -6551,7 +6560,7 @@
       <c r="U95" s="6"/>
       <c r="V95" s="6"/>
     </row>
-    <row r="96" ht="14.8">
+    <row r="96" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A96" s="3">
         <v>991365614</v>
       </c>
@@ -6599,7 +6608,7 @@
       <c r="U96" s="6"/>
       <c r="V96" s="6"/>
     </row>
-    <row r="97" ht="14.8">
+    <row r="97" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A97" s="3">
         <v>991365965</v>
       </c>
@@ -6647,7 +6656,7 @@
       <c r="U97" s="6"/>
       <c r="V97" s="6"/>
     </row>
-    <row r="98" ht="14.8">
+    <row r="98" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A98" s="3">
         <v>991366045</v>
       </c>
@@ -6699,7 +6708,7 @@
       <c r="U98" s="6"/>
       <c r="V98" s="6"/>
     </row>
-    <row r="99" ht="14.8">
+    <row r="99" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A99" s="3">
         <v>991366116</v>
       </c>
@@ -6747,7 +6756,7 @@
       <c r="U99" s="6"/>
       <c r="V99" s="6"/>
     </row>
-    <row r="100" ht="14.8">
+    <row r="100" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A100" s="3">
         <v>991366549</v>
       </c>
@@ -6795,7 +6804,7 @@
       <c r="U100" s="6"/>
       <c r="V100" s="6"/>
     </row>
-    <row r="101" ht="14.8">
+    <row r="101" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A101" s="3">
         <v>991366987</v>
       </c>
@@ -6843,7 +6852,7 @@
       <c r="U101" s="6"/>
       <c r="V101" s="6"/>
     </row>
-    <row r="102" ht="14.8">
+    <row r="102" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A102" s="3">
         <v>991370707</v>
       </c>
@@ -6891,7 +6900,7 @@
       <c r="U102" s="6"/>
       <c r="V102" s="6"/>
     </row>
-    <row r="103" ht="14.8">
+    <row r="103" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A103" s="3">
         <v>991370730</v>
       </c>
@@ -6939,7 +6948,7 @@
       <c r="U103" s="6"/>
       <c r="V103" s="6"/>
     </row>
-    <row r="104" ht="14.8">
+    <row r="104" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A104" s="3">
         <v>991370743</v>
       </c>
@@ -6987,7 +6996,7 @@
       <c r="U104" s="6"/>
       <c r="V104" s="6"/>
     </row>
-    <row r="105" ht="14.8">
+    <row r="105" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A105" s="3">
         <v>991370750</v>
       </c>
@@ -7035,7 +7044,7 @@
       <c r="U105" s="6"/>
       <c r="V105" s="6"/>
     </row>
-    <row r="106" ht="14.8">
+    <row r="106" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A106" s="3">
         <v>991370767</v>
       </c>
@@ -7083,7 +7092,7 @@
       <c r="U106" s="6"/>
       <c r="V106" s="6"/>
     </row>
-    <row r="107" ht="14.8">
+    <row r="107" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A107" s="3">
         <v>991370781</v>
       </c>
@@ -7131,7 +7140,7 @@
       <c r="U107" s="6"/>
       <c r="V107" s="6"/>
     </row>
-    <row r="108" ht="28.25">
+    <row r="108" spans="1:22" ht="29" x14ac:dyDescent="0.35">
       <c r="A108" s="3">
         <v>991372132</v>
       </c>
@@ -7179,7 +7188,7 @@
       <c r="U108" s="6"/>
       <c r="V108" s="6"/>
     </row>
-    <row r="109" ht="28.25">
+    <row r="109" spans="1:22" ht="29" x14ac:dyDescent="0.35">
       <c r="A109" s="3">
         <v>991372144</v>
       </c>
@@ -7227,7 +7236,7 @@
       <c r="U109" s="6"/>
       <c r="V109" s="6"/>
     </row>
-    <row r="110" ht="14.8">
+    <row r="110" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A110" s="3">
         <v>991395089</v>
       </c>
@@ -7275,7 +7284,7 @@
       <c r="U110" s="6"/>
       <c r="V110" s="6"/>
     </row>
-    <row r="111" ht="14.8">
+    <row r="111" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A111" s="3">
         <v>991404604</v>
       </c>
@@ -7323,7 +7332,7 @@
       <c r="U111" s="6"/>
       <c r="V111" s="6"/>
     </row>
-    <row r="112" ht="14.8">
+    <row r="112" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A112" s="3">
         <v>991404759</v>
       </c>
@@ -7371,7 +7380,7 @@
       <c r="U112" s="6"/>
       <c r="V112" s="6"/>
     </row>
-    <row r="113" ht="14.8">
+    <row r="113" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A113" s="3">
         <v>991510905</v>
       </c>
@@ -7419,7 +7428,7 @@
       <c r="U113" s="6"/>
       <c r="V113" s="6"/>
     </row>
-    <row r="114" ht="14.8">
+    <row r="114" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A114" s="3">
         <v>991511155</v>
       </c>
@@ -7459,7 +7468,7 @@
       <c r="U114" s="6"/>
       <c r="V114" s="6"/>
     </row>
-    <row r="115" ht="14.8">
+    <row r="115" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A115" s="3">
         <v>991524355</v>
       </c>
@@ -7507,7 +7516,7 @@
       <c r="U115" s="6"/>
       <c r="V115" s="6"/>
     </row>
-    <row r="116" ht="14.8">
+    <row r="116" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A116" s="3">
         <v>991583092</v>
       </c>
@@ -7555,7 +7564,7 @@
       <c r="U116" s="6"/>
       <c r="V116" s="6"/>
     </row>
-    <row r="117" ht="14.8">
+    <row r="117" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A117" s="3">
         <v>991590081</v>
       </c>
@@ -7603,7 +7612,7 @@
       <c r="U117" s="6"/>
       <c r="V117" s="6"/>
     </row>
-    <row r="118" ht="14.8">
+    <row r="118" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A118" s="3">
         <v>991590297</v>
       </c>
@@ -7651,7 +7660,7 @@
       <c r="U118" s="6"/>
       <c r="V118" s="6"/>
     </row>
-    <row r="119" ht="14.8">
+    <row r="119" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A119" s="3">
         <v>991590450</v>
       </c>
@@ -7699,7 +7708,7 @@
       <c r="U119" s="6"/>
       <c r="V119" s="6"/>
     </row>
-    <row r="120" ht="14.8">
+    <row r="120" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A120" s="3">
         <v>991590491</v>
       </c>
@@ -7747,7 +7756,7 @@
       <c r="U120" s="6"/>
       <c r="V120" s="6"/>
     </row>
-    <row r="121" ht="14.8">
+    <row r="121" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A121" s="3">
         <v>991590644</v>
       </c>
@@ -7795,7 +7804,7 @@
       <c r="U121" s="6"/>
       <c r="V121" s="6"/>
     </row>
-    <row r="122" ht="14.8">
+    <row r="122" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A122" s="3">
         <v>991590773</v>
       </c>
@@ -7843,7 +7852,7 @@
       <c r="U122" s="6"/>
       <c r="V122" s="6"/>
     </row>
-    <row r="123" ht="14.8">
+    <row r="123" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A123" s="3">
         <v>991591678</v>
       </c>
@@ -7891,7 +7900,7 @@
       <c r="U123" s="6"/>
       <c r="V123" s="6"/>
     </row>
-    <row r="124" ht="14.8">
+    <row r="124" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A124" s="3">
         <v>991591972</v>
       </c>
@@ -7939,7 +7948,7 @@
       <c r="U124" s="6"/>
       <c r="V124" s="6"/>
     </row>
-    <row r="125" ht="14.8">
+    <row r="125" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A125" s="3">
         <v>991592038</v>
       </c>
@@ -7991,7 +8000,7 @@
       <c r="U125" s="6"/>
       <c r="V125" s="6"/>
     </row>
-    <row r="126" ht="14.8">
+    <row r="126" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A126" s="3">
         <v>991592061</v>
       </c>
@@ -8043,7 +8052,7 @@
       <c r="U126" s="6"/>
       <c r="V126" s="6"/>
     </row>
-    <row r="127" ht="14.8">
+    <row r="127" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A127" s="3">
         <v>991592830</v>
       </c>
@@ -8091,7 +8100,7 @@
       <c r="U127" s="6"/>
       <c r="V127" s="6"/>
     </row>
-    <row r="128" ht="14.8">
+    <row r="128" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A128" s="3">
         <v>991592845</v>
       </c>
@@ -8139,7 +8148,7 @@
       <c r="U128" s="6"/>
       <c r="V128" s="6"/>
     </row>
-    <row r="129" ht="14.8">
+    <row r="129" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A129" s="3">
         <v>991592965</v>
       </c>
@@ -8187,7 +8196,7 @@
       <c r="U129" s="6"/>
       <c r="V129" s="6"/>
     </row>
-    <row r="130" ht="14.8">
+    <row r="130" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A130" s="3">
         <v>991593336</v>
       </c>
@@ -8227,7 +8236,7 @@
       <c r="U130" s="6"/>
       <c r="V130" s="6"/>
     </row>
-    <row r="131" ht="28.25">
+    <row r="131" spans="1:22" ht="29" x14ac:dyDescent="0.35">
       <c r="A131" s="3">
         <v>991593915</v>
       </c>
@@ -8275,7 +8284,7 @@
       <c r="U131" s="6"/>
       <c r="V131" s="6"/>
     </row>
-    <row r="132" ht="28.25">
+    <row r="132" spans="1:22" ht="29" x14ac:dyDescent="0.35">
       <c r="A132" s="3">
         <v>991594100</v>
       </c>
@@ -8323,7 +8332,7 @@
       <c r="U132" s="6"/>
       <c r="V132" s="6"/>
     </row>
-    <row r="133" ht="14.8">
+    <row r="133" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A133" s="3">
         <v>991596961</v>
       </c>
@@ -8363,7 +8372,7 @@
       <c r="U133" s="6"/>
       <c r="V133" s="6"/>
     </row>
-    <row r="134" ht="41.65">
+    <row r="134" spans="1:22" ht="29" x14ac:dyDescent="0.35">
       <c r="A134" s="3">
         <v>991597001</v>
       </c>
@@ -8411,7 +8420,7 @@
       <c r="U134" s="6"/>
       <c r="V134" s="6"/>
     </row>
-    <row r="135" ht="14.8">
+    <row r="135" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A135" s="3">
         <v>991606959</v>
       </c>
@@ -8459,7 +8468,7 @@
       <c r="U135" s="6"/>
       <c r="V135" s="6"/>
     </row>
-    <row r="136" ht="14.8">
+    <row r="136" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A136" s="3">
         <v>991607204</v>
       </c>
@@ -8507,7 +8516,7 @@
       <c r="U136" s="6"/>
       <c r="V136" s="6"/>
     </row>
-    <row r="137" ht="14.8">
+    <row r="137" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A137" s="3">
         <v>991612561</v>
       </c>
@@ -8555,7 +8564,7 @@
       <c r="U137" s="6"/>
       <c r="V137" s="6"/>
     </row>
-    <row r="138" ht="14.8">
+    <row r="138" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A138" s="3">
         <v>991612716</v>
       </c>
@@ -8595,7 +8604,7 @@
       <c r="U138" s="6"/>
       <c r="V138" s="6"/>
     </row>
-    <row r="139" ht="14.8">
+    <row r="139" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A139" s="3">
         <v>991613100</v>
       </c>
@@ -8647,7 +8656,7 @@
       <c r="U139" s="6"/>
       <c r="V139" s="6"/>
     </row>
-    <row r="140" ht="14.8">
+    <row r="140" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A140" s="3">
         <v>991630545</v>
       </c>
@@ -8695,7 +8704,7 @@
       <c r="U140" s="6"/>
       <c r="V140" s="6"/>
     </row>
-    <row r="141" ht="14.8">
+    <row r="141" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A141" s="3">
         <v>991630727</v>
       </c>
@@ -8743,7 +8752,7 @@
       <c r="U141" s="6"/>
       <c r="V141" s="6"/>
     </row>
-    <row r="142" ht="28.25">
+    <row r="142" spans="1:22" ht="29" x14ac:dyDescent="0.35">
       <c r="A142" s="3">
         <v>991632142</v>
       </c>
@@ -8791,7 +8800,7 @@
       <c r="U142" s="6"/>
       <c r="V142" s="6"/>
     </row>
-    <row r="143" ht="14.8">
+    <row r="143" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A143" s="3">
         <v>991635671</v>
       </c>
@@ -8839,7 +8848,7 @@
       <c r="U143" s="6"/>
       <c r="V143" s="6"/>
     </row>
-    <row r="144" ht="14.8">
+    <row r="144" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A144" s="3">
         <v>991651718</v>
       </c>
@@ -8887,7 +8896,7 @@
       <c r="U144" s="6"/>
       <c r="V144" s="6"/>
     </row>
-    <row r="145" ht="14.8">
+    <row r="145" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A145" s="3">
         <v>991652008</v>
       </c>
@@ -8935,7 +8944,7 @@
       <c r="U145" s="6"/>
       <c r="V145" s="6"/>
     </row>
-    <row r="146" ht="14.8">
+    <row r="146" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A146" s="3">
         <v>991652656</v>
       </c>
@@ -8983,7 +8992,7 @@
       <c r="U146" s="6"/>
       <c r="V146" s="6"/>
     </row>
-    <row r="147" ht="14.8">
+    <row r="147" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A147" s="3">
         <v>991653036</v>
       </c>
@@ -9031,7 +9040,7 @@
       <c r="U147" s="6"/>
       <c r="V147" s="6"/>
     </row>
-    <row r="148" ht="14.8">
+    <row r="148" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A148" s="3">
         <v>991653254</v>
       </c>
@@ -9079,7 +9088,7 @@
       <c r="U148" s="6"/>
       <c r="V148" s="6"/>
     </row>
-    <row r="149" ht="14.8">
+    <row r="149" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A149" s="3">
         <v>991653272</v>
       </c>
@@ -9127,7 +9136,7 @@
       <c r="U149" s="6"/>
       <c r="V149" s="6"/>
     </row>
-    <row r="150" ht="14.8">
+    <row r="150" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A150" s="3">
         <v>991678758</v>
       </c>
@@ -9167,7 +9176,7 @@
       <c r="U150" s="6"/>
       <c r="V150" s="6"/>
     </row>
-    <row r="151" ht="14.8">
+    <row r="151" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A151" s="3">
         <v>991679196</v>
       </c>
@@ -9215,7 +9224,7 @@
       <c r="U151" s="6"/>
       <c r="V151" s="6"/>
     </row>
-    <row r="152" ht="14.8">
+    <row r="152" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A152" s="3">
         <v>991679305</v>
       </c>
@@ -9263,7 +9272,7 @@
       <c r="U152" s="6"/>
       <c r="V152" s="6"/>
     </row>
-    <row r="153" ht="14.8">
+    <row r="153" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A153" s="3">
         <v>991679692</v>
       </c>
@@ -9309,7 +9318,7 @@
       <c r="U153" s="6"/>
       <c r="V153" s="6"/>
     </row>
-    <row r="154" ht="14.8">
+    <row r="154" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A154" s="3">
         <v>991679698</v>
       </c>
@@ -9357,7 +9366,7 @@
       <c r="U154" s="6"/>
       <c r="V154" s="6"/>
     </row>
-    <row r="155" ht="14.8">
+    <row r="155" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A155" s="3">
         <v>991679708</v>
       </c>
@@ -9405,7 +9414,7 @@
       <c r="U155" s="6"/>
       <c r="V155" s="6"/>
     </row>
-    <row r="156" ht="14.8">
+    <row r="156" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A156" s="3">
         <v>991680498</v>
       </c>
@@ -9453,7 +9462,7 @@
       <c r="U156" s="6"/>
       <c r="V156" s="6"/>
     </row>
-    <row r="157" ht="14.8">
+    <row r="157" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A157" s="3">
         <v>991680841</v>
       </c>
@@ -9501,7 +9510,7 @@
       <c r="U157" s="6"/>
       <c r="V157" s="6"/>
     </row>
-    <row r="158" ht="14.8">
+    <row r="158" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A158" s="3">
         <v>991681840</v>
       </c>
@@ -9549,7 +9558,7 @@
       <c r="U158" s="6"/>
       <c r="V158" s="6"/>
     </row>
-    <row r="159" ht="14.8">
+    <row r="159" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A159" s="3">
         <v>991681860</v>
       </c>
@@ -9597,7 +9606,7 @@
       <c r="U159" s="6"/>
       <c r="V159" s="6"/>
     </row>
-    <row r="160" ht="14.8">
+    <row r="160" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A160" s="3">
         <v>991682062</v>
       </c>
@@ -9645,7 +9654,7 @@
       <c r="U160" s="6"/>
       <c r="V160" s="6"/>
     </row>
-    <row r="161" ht="14.8">
+    <row r="161" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A161" s="3">
         <v>991682097</v>
       </c>
@@ -9693,7 +9702,7 @@
       <c r="U161" s="6"/>
       <c r="V161" s="6"/>
     </row>
-    <row r="162" ht="14.8">
+    <row r="162" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A162" s="3">
         <v>991682854</v>
       </c>
@@ -9741,7 +9750,7 @@
       <c r="U162" s="6"/>
       <c r="V162" s="6"/>
     </row>
-    <row r="163" ht="14.8">
+    <row r="163" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A163" s="3">
         <v>991682887</v>
       </c>
@@ -9789,7 +9798,7 @@
       <c r="U163" s="6"/>
       <c r="V163" s="6"/>
     </row>
-    <row r="164" ht="14.8">
+    <row r="164" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A164" s="3">
         <v>991682998</v>
       </c>
@@ -9837,7 +9846,7 @@
       <c r="U164" s="6"/>
       <c r="V164" s="6"/>
     </row>
-    <row r="165" ht="28.25">
+    <row r="165" spans="1:22" ht="29" x14ac:dyDescent="0.35">
       <c r="A165" s="3">
         <v>991684632</v>
       </c>
@@ -9885,7 +9894,7 @@
       <c r="U165" s="6"/>
       <c r="V165" s="6"/>
     </row>
-    <row r="166" ht="14.8">
+    <row r="166" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A166" s="3">
         <v>991686066</v>
       </c>
@@ -9933,7 +9942,7 @@
       <c r="U166" s="6"/>
       <c r="V166" s="6"/>
     </row>
-    <row r="167" ht="14.8">
+    <row r="167" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A167" s="3">
         <v>991686093</v>
       </c>
@@ -9981,7 +9990,7 @@
       <c r="U167" s="6"/>
       <c r="V167" s="6"/>
     </row>
-    <row r="168" ht="14.8">
+    <row r="168" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A168" s="3">
         <v>991686181</v>
       </c>
@@ -10029,7 +10038,7 @@
       <c r="U168" s="6"/>
       <c r="V168" s="6"/>
     </row>
-    <row r="169" ht="14.8">
+    <row r="169" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A169" s="3">
         <v>991686192</v>
       </c>
@@ -10081,7 +10090,7 @@
       <c r="U169" s="6"/>
       <c r="V169" s="6"/>
     </row>
-    <row r="170" ht="28.25">
+    <row r="170" spans="1:22" ht="29" x14ac:dyDescent="0.35">
       <c r="A170" s="3">
         <v>991686264</v>
       </c>
@@ -10129,7 +10138,7 @@
       <c r="U170" s="6"/>
       <c r="V170" s="6"/>
     </row>
-    <row r="171" ht="28.25">
+    <row r="171" spans="1:22" ht="29" x14ac:dyDescent="0.35">
       <c r="A171" s="3">
         <v>991686341</v>
       </c>
@@ -10189,7 +10198,7 @@
       <c r="U171" s="6"/>
       <c r="V171" s="6"/>
     </row>
-    <row r="172" ht="14.8">
+    <row r="172" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A172" s="3">
         <v>991686378</v>
       </c>
@@ -10237,7 +10246,7 @@
       <c r="U172" s="6"/>
       <c r="V172" s="6"/>
     </row>
-    <row r="173" ht="14.8">
+    <row r="173" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A173" s="3">
         <v>991686489</v>
       </c>
@@ -10285,7 +10294,7 @@
       <c r="U173" s="6"/>
       <c r="V173" s="6"/>
     </row>
-    <row r="174" ht="14.8">
+    <row r="174" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A174" s="3">
         <v>991687649</v>
       </c>
@@ -10333,7 +10342,7 @@
       <c r="U174" s="6"/>
       <c r="V174" s="6"/>
     </row>
-    <row r="175" ht="14.8">
+    <row r="175" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A175" s="3">
         <v>991688142</v>
       </c>
@@ -10381,7 +10390,7 @@
       <c r="U175" s="6"/>
       <c r="V175" s="6"/>
     </row>
-    <row r="176" ht="14.8">
+    <row r="176" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A176" s="3">
         <v>991688374</v>
       </c>
@@ -10429,7 +10438,7 @@
       <c r="U176" s="6"/>
       <c r="V176" s="6"/>
     </row>
-    <row r="177" ht="14.8">
+    <row r="177" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A177" s="3">
         <v>991688623</v>
       </c>
@@ -10477,7 +10486,7 @@
       <c r="U177" s="6"/>
       <c r="V177" s="6"/>
     </row>
-    <row r="178" ht="14.8">
+    <row r="178" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A178" s="3">
         <v>991689565</v>
       </c>
@@ -10525,7 +10534,7 @@
       <c r="U178" s="6"/>
       <c r="V178" s="6"/>
     </row>
-    <row r="179" ht="14.8">
+    <row r="179" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A179" s="3">
         <v>991689793</v>
       </c>
@@ -10573,7 +10582,7 @@
       <c r="U179" s="6"/>
       <c r="V179" s="6"/>
     </row>
-    <row r="180" ht="14.8">
+    <row r="180" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A180" s="3">
         <v>991689953</v>
       </c>
@@ -10613,7 +10622,7 @@
       <c r="U180" s="6"/>
       <c r="V180" s="6"/>
     </row>
-    <row r="181" ht="28.25">
+    <row r="181" spans="1:22" ht="29" x14ac:dyDescent="0.35">
       <c r="A181" s="3">
         <v>991690058</v>
       </c>
@@ -10661,7 +10670,7 @@
       <c r="U181" s="6"/>
       <c r="V181" s="6"/>
     </row>
-    <row r="182" ht="28.25">
+    <row r="182" spans="1:22" ht="29" x14ac:dyDescent="0.35">
       <c r="A182" s="3">
         <v>991690085</v>
       </c>
@@ -10709,7 +10718,7 @@
       <c r="U182" s="6"/>
       <c r="V182" s="6"/>
     </row>
-    <row r="183" ht="14.8">
+    <row r="183" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A183" s="3">
         <v>991690118</v>
       </c>
@@ -10757,7 +10766,7 @@
       <c r="U183" s="6"/>
       <c r="V183" s="6"/>
     </row>
-    <row r="184" ht="14.8">
+    <row r="184" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A184" s="3">
         <v>991690133</v>
       </c>
@@ -10805,7 +10814,7 @@
       <c r="U184" s="6"/>
       <c r="V184" s="6"/>
     </row>
-    <row r="185" ht="14.8">
+    <row r="185" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A185" s="3">
         <v>991715208</v>
       </c>
@@ -10853,7 +10862,7 @@
       <c r="U185" s="6"/>
       <c r="V185" s="6"/>
     </row>
-    <row r="186" ht="14.8">
+    <row r="186" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A186" s="3">
         <v>991715216</v>
       </c>
@@ -10901,7 +10910,7 @@
       <c r="U186" s="6"/>
       <c r="V186" s="6"/>
     </row>
-    <row r="187" ht="14.8">
+    <row r="187" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A187" s="3">
         <v>991715972</v>
       </c>
@@ -10949,7 +10958,7 @@
       <c r="U187" s="6"/>
       <c r="V187" s="6"/>
     </row>
-    <row r="188" ht="28.25">
+    <row r="188" spans="1:22" ht="29" x14ac:dyDescent="0.35">
       <c r="A188" s="3">
         <v>991719442</v>
       </c>
@@ -10997,7 +11006,7 @@
       <c r="U188" s="6"/>
       <c r="V188" s="6"/>
     </row>
-    <row r="189" ht="14.8">
+    <row r="189" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A189" s="3">
         <v>991719680</v>
       </c>
@@ -11045,7 +11054,7 @@
       <c r="U189" s="6"/>
       <c r="V189" s="6"/>
     </row>
-    <row r="190" ht="14.8">
+    <row r="190" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A190" s="3">
         <v>991720517</v>
       </c>
@@ -11093,7 +11102,7 @@
       <c r="U190" s="6"/>
       <c r="V190" s="6"/>
     </row>
-    <row r="191" ht="14.8">
+    <row r="191" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A191" s="3">
         <v>991721849</v>
       </c>
@@ -11141,7 +11150,7 @@
       <c r="U191" s="6"/>
       <c r="V191" s="6"/>
     </row>
-    <row r="192" ht="14.8">
+    <row r="192" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A192" s="3">
         <v>991723065</v>
       </c>
@@ -11189,7 +11198,7 @@
       <c r="U192" s="6"/>
       <c r="V192" s="6"/>
     </row>
-    <row r="193" ht="28.25">
+    <row r="193" spans="1:22" ht="29" x14ac:dyDescent="0.35">
       <c r="A193" s="3">
         <v>991723261</v>
       </c>
@@ -11237,7 +11246,7 @@
       <c r="U193" s="6"/>
       <c r="V193" s="6"/>
     </row>
-    <row r="194" ht="14.8">
+    <row r="194" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A194" s="3">
         <v>991724359</v>
       </c>
@@ -11285,7 +11294,7 @@
       <c r="U194" s="6"/>
       <c r="V194" s="6"/>
     </row>
-    <row r="195" ht="14.8">
+    <row r="195" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A195" s="3">
         <v>991724964</v>
       </c>
@@ -11333,7 +11342,7 @@
       <c r="U195" s="6"/>
       <c r="V195" s="6"/>
     </row>
-    <row r="196" ht="14.8">
+    <row r="196" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A196" s="3">
         <v>991725109</v>
       </c>
@@ -11373,7 +11382,7 @@
       <c r="U196" s="6"/>
       <c r="V196" s="6"/>
     </row>
-    <row r="197" ht="14.8">
+    <row r="197" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A197" s="3">
         <v>991725113</v>
       </c>
@@ -11413,7 +11422,7 @@
       <c r="U197" s="6"/>
       <c r="V197" s="6"/>
     </row>
-    <row r="198" ht="14.8">
+    <row r="198" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A198" s="3">
         <v>991725143</v>
       </c>
@@ -11461,7 +11470,7 @@
       <c r="U198" s="6"/>
       <c r="V198" s="6"/>
     </row>
-    <row r="199" ht="14.8">
+    <row r="199" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A199" s="3">
         <v>991731003</v>
       </c>
@@ -11509,7 +11518,7 @@
       <c r="U199" s="6"/>
       <c r="V199" s="6"/>
     </row>
-    <row r="200" ht="14.8">
+    <row r="200" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A200" s="3">
         <v>991731027</v>
       </c>
@@ -11549,7 +11558,7 @@
       <c r="U200" s="6"/>
       <c r="V200" s="6"/>
     </row>
-    <row r="201" ht="14.8">
+    <row r="201" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A201" s="3">
         <v>991731035</v>
       </c>
@@ -11589,7 +11598,7 @@
       <c r="U201" s="6"/>
       <c r="V201" s="6"/>
     </row>
-    <row r="202" ht="14.8">
+    <row r="202" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A202" s="3">
         <v>991731150</v>
       </c>
@@ -11637,7 +11646,7 @@
       <c r="U202" s="6"/>
       <c r="V202" s="6"/>
     </row>
-    <row r="203" ht="14.8">
+    <row r="203" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A203" s="3">
         <v>991731520</v>
       </c>
@@ -11677,7 +11686,7 @@
       <c r="U203" s="6"/>
       <c r="V203" s="6"/>
     </row>
-    <row r="204" ht="14.8">
+    <row r="204" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A204" s="3">
         <v>991731732</v>
       </c>
@@ -11725,7 +11734,7 @@
       <c r="U204" s="6"/>
       <c r="V204" s="6"/>
     </row>
-    <row r="205" ht="14.8">
+    <row r="205" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A205" s="3">
         <v>991732889</v>
       </c>
@@ -11773,7 +11782,7 @@
       <c r="U205" s="6"/>
       <c r="V205" s="6"/>
     </row>
-    <row r="206" ht="14.8">
+    <row r="206" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A206" s="3">
         <v>991732929</v>
       </c>
@@ -11821,7 +11830,7 @@
       <c r="U206" s="6"/>
       <c r="V206" s="6"/>
     </row>
-    <row r="207" ht="14.8">
+    <row r="207" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A207" s="3">
         <v>991733530</v>
       </c>
@@ -11869,7 +11878,7 @@
       <c r="U207" s="6"/>
       <c r="V207" s="6"/>
     </row>
-    <row r="208" ht="14.8">
+    <row r="208" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A208" s="3">
         <v>991733623</v>
       </c>
@@ -11917,7 +11926,7 @@
       <c r="U208" s="6"/>
       <c r="V208" s="6"/>
     </row>
-    <row r="209" ht="14.8">
+    <row r="209" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A209" s="3">
         <v>991733955</v>
       </c>
@@ -11965,7 +11974,7 @@
       <c r="U209" s="6"/>
       <c r="V209" s="6"/>
     </row>
-    <row r="210" ht="14.8">
+    <row r="210" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A210" s="3">
         <v>991735462</v>
       </c>
@@ -12005,7 +12014,7 @@
       <c r="U210" s="6"/>
       <c r="V210" s="6"/>
     </row>
-    <row r="211" ht="14.8">
+    <row r="211" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A211" s="3">
         <v>991735720</v>
       </c>
@@ -12051,7 +12060,7 @@
       <c r="U211" s="6"/>
       <c r="V211" s="6"/>
     </row>
-    <row r="212" ht="14.8">
+    <row r="212" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A212" s="3">
         <v>991736334</v>
       </c>
@@ -12099,7 +12108,7 @@
       <c r="U212" s="6"/>
       <c r="V212" s="6"/>
     </row>
-    <row r="213" ht="14.8">
+    <row r="213" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A213" s="3">
         <v>991736572</v>
       </c>
@@ -12147,7 +12156,7 @@
       <c r="U213" s="6"/>
       <c r="V213" s="6"/>
     </row>
-    <row r="214" ht="14.8">
+    <row r="214" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A214" s="3">
         <v>991736902</v>
       </c>
@@ -12187,7 +12196,7 @@
       <c r="U214" s="6"/>
       <c r="V214" s="6"/>
     </row>
-    <row r="215" ht="14.8">
+    <row r="215" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A215" s="3">
         <v>991737315</v>
       </c>
@@ -12235,7 +12244,7 @@
       <c r="U215" s="6"/>
       <c r="V215" s="6"/>
     </row>
-    <row r="216" ht="14.8">
+    <row r="216" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A216" s="3">
         <v>991741711</v>
       </c>
@@ -12283,7 +12292,7 @@
       <c r="U216" s="6"/>
       <c r="V216" s="6"/>
     </row>
-    <row r="217" ht="14.8">
+    <row r="217" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A217" s="3">
         <v>991741978</v>
       </c>
@@ -12331,7 +12340,7 @@
       <c r="U217" s="6"/>
       <c r="V217" s="6"/>
     </row>
-    <row r="218" ht="14.8">
+    <row r="218" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A218" s="3">
         <v>991742010</v>
       </c>
@@ -12379,7 +12388,7 @@
       <c r="U218" s="6"/>
       <c r="V218" s="6"/>
     </row>
-    <row r="219" ht="14.8">
+    <row r="219" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A219" s="3">
         <v>991742155</v>
       </c>
@@ -12427,7 +12436,7 @@
       <c r="U219" s="6"/>
       <c r="V219" s="6"/>
     </row>
-    <row r="220" ht="14.8">
+    <row r="220" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A220" s="3">
         <v>991742229</v>
       </c>
@@ -12475,7 +12484,7 @@
       <c r="U220" s="6"/>
       <c r="V220" s="6"/>
     </row>
-    <row r="221" ht="14.8">
+    <row r="221" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A221" s="3">
         <v>991742334</v>
       </c>
@@ -12523,7 +12532,7 @@
       <c r="U221" s="6"/>
       <c r="V221" s="6"/>
     </row>
-    <row r="222" ht="14.8">
+    <row r="222" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A222" s="3">
         <v>991742855</v>
       </c>
@@ -12571,7 +12580,7 @@
       <c r="U222" s="6"/>
       <c r="V222" s="6"/>
     </row>
-    <row r="223" ht="28.25">
+    <row r="223" spans="1:22" ht="29" x14ac:dyDescent="0.35">
       <c r="A223" s="3">
         <v>991744524</v>
       </c>
@@ -12619,7 +12628,7 @@
       <c r="U223" s="6"/>
       <c r="V223" s="6"/>
     </row>
-    <row r="224" ht="14.8">
+    <row r="224" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A224" s="3">
         <v>991745097</v>
       </c>
@@ -12667,7 +12676,7 @@
       <c r="U224" s="6"/>
       <c r="V224" s="6"/>
     </row>
-    <row r="225" ht="14.8">
+    <row r="225" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A225" s="3">
         <v>991746834</v>
       </c>
@@ -12715,7 +12724,7 @@
       <c r="U225" s="6"/>
       <c r="V225" s="6"/>
     </row>
-    <row r="226" ht="14.8">
+    <row r="226" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A226" s="3">
         <v>991747890</v>
       </c>
@@ -12763,7 +12772,7 @@
       <c r="U226" s="6"/>
       <c r="V226" s="6"/>
     </row>
-    <row r="227" ht="14.8">
+    <row r="227" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A227" s="3">
         <v>991748107</v>
       </c>
@@ -12803,7 +12812,7 @@
       <c r="U227" s="6"/>
       <c r="V227" s="6"/>
     </row>
-    <row r="228" ht="14.8">
+    <row r="228" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A228" s="3">
         <v>991748996</v>
       </c>
@@ -12851,7 +12860,7 @@
       <c r="U228" s="6"/>
       <c r="V228" s="6"/>
     </row>
-    <row r="229" ht="14.8">
+    <row r="229" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A229" s="3">
         <v>991749068</v>
       </c>
@@ -12891,7 +12900,7 @@
       <c r="U229" s="6"/>
       <c r="V229" s="6"/>
     </row>
-    <row r="230" ht="14.8">
+    <row r="230" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A230" s="3">
         <v>991752009</v>
       </c>
@@ -12939,7 +12948,7 @@
       <c r="U230" s="6"/>
       <c r="V230" s="6"/>
     </row>
-    <row r="231" ht="14.8">
+    <row r="231" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A231" s="3">
         <v>991752417</v>
       </c>
@@ -12987,7 +12996,7 @@
       <c r="U231" s="6"/>
       <c r="V231" s="6"/>
     </row>
-    <row r="232" ht="14.8">
+    <row r="232" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A232" s="3">
         <v>991752569</v>
       </c>
@@ -13027,7 +13036,7 @@
       <c r="U232" s="6"/>
       <c r="V232" s="6"/>
     </row>
-    <row r="233" ht="14.8">
+    <row r="233" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A233" s="3">
         <v>991752663</v>
       </c>
@@ -13075,7 +13084,7 @@
       <c r="U233" s="6"/>
       <c r="V233" s="6"/>
     </row>
-    <row r="234" ht="14.8">
+    <row r="234" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A234" s="3">
         <v>991753155</v>
       </c>
@@ -13123,7 +13132,7 @@
       <c r="U234" s="6"/>
       <c r="V234" s="6"/>
     </row>
-    <row r="235" ht="28.25">
+    <row r="235" spans="1:22" ht="29" x14ac:dyDescent="0.35">
       <c r="A235" s="3">
         <v>991753363</v>
       </c>
@@ -13183,7 +13192,7 @@
       <c r="U235" s="6"/>
       <c r="V235" s="6"/>
     </row>
-    <row r="236" ht="28.25">
+    <row r="236" spans="1:22" ht="29" x14ac:dyDescent="0.35">
       <c r="A236" s="3">
         <v>991753387</v>
       </c>
@@ -13243,7 +13252,7 @@
       <c r="U236" s="6"/>
       <c r="V236" s="6"/>
     </row>
-    <row r="237" ht="28.25">
+    <row r="237" spans="1:22" ht="29" x14ac:dyDescent="0.35">
       <c r="A237" s="3">
         <v>991753853</v>
       </c>
@@ -13291,7 +13300,7 @@
       <c r="U237" s="6"/>
       <c r="V237" s="6"/>
     </row>
-    <row r="238" ht="14.8">
+    <row r="238" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A238" s="3">
         <v>991753882</v>
       </c>
@@ -13339,7 +13348,7 @@
       <c r="U238" s="6"/>
       <c r="V238" s="6"/>
     </row>
-    <row r="239" ht="14.8">
+    <row r="239" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A239" s="3">
         <v>991754084</v>
       </c>
@@ -13387,7 +13396,7 @@
       <c r="U239" s="6"/>
       <c r="V239" s="6"/>
     </row>
-    <row r="240" ht="14.8">
+    <row r="240" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A240" s="3">
         <v>991754513</v>
       </c>
@@ -13435,7 +13444,7 @@
       <c r="U240" s="6"/>
       <c r="V240" s="6"/>
     </row>
-    <row r="241" ht="14.8">
+    <row r="241" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A241" s="3">
         <v>991755677</v>
       </c>
@@ -13483,7 +13492,7 @@
       <c r="U241" s="6"/>
       <c r="V241" s="6"/>
     </row>
-    <row r="242" ht="14.8">
+    <row r="242" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A242" s="3">
         <v>991755678</v>
       </c>
@@ -13531,7 +13540,7 @@
       <c r="U242" s="6"/>
       <c r="V242" s="6"/>
     </row>
-    <row r="243" ht="14.8">
+    <row r="243" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A243" s="3">
         <v>991755713</v>
       </c>
@@ -13571,7 +13580,7 @@
       <c r="U243" s="6"/>
       <c r="V243" s="6"/>
     </row>
-    <row r="244" ht="14.8">
+    <row r="244" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A244" s="3">
         <v>991755916</v>
       </c>
@@ -13619,7 +13628,7 @@
       <c r="U244" s="6"/>
       <c r="V244" s="6"/>
     </row>
-    <row r="245" ht="14.8">
+    <row r="245" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A245" s="3">
         <v>991790621</v>
       </c>
@@ -13667,7 +13676,7 @@
       <c r="U245" s="6"/>
       <c r="V245" s="6"/>
     </row>
-    <row r="246" ht="14.8">
+    <row r="246" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A246" s="3">
         <v>991791213</v>
       </c>
@@ -13715,7 +13724,7 @@
       <c r="U246" s="6"/>
       <c r="V246" s="6"/>
     </row>
-    <row r="247" ht="14.8">
+    <row r="247" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A247" s="3">
         <v>991792121</v>
       </c>
@@ -13775,7 +13784,7 @@
       <c r="U247" s="6"/>
       <c r="V247" s="6"/>
     </row>
-    <row r="248" ht="28.25">
+    <row r="248" spans="1:22" ht="29" x14ac:dyDescent="0.35">
       <c r="A248" s="3">
         <v>991792227</v>
       </c>
@@ -13823,7 +13832,7 @@
       <c r="U248" s="6"/>
       <c r="V248" s="6"/>
     </row>
-    <row r="249" ht="14.8">
+    <row r="249" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A249" s="3">
         <v>991792232</v>
       </c>
@@ -13871,7 +13880,7 @@
       <c r="U249" s="6"/>
       <c r="V249" s="6"/>
     </row>
-    <row r="250" ht="14.8">
+    <row r="250" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A250" s="3">
         <v>991824591</v>
       </c>
@@ -13919,7 +13928,7 @@
       <c r="U250" s="6"/>
       <c r="V250" s="6"/>
     </row>
-    <row r="251" ht="14.8">
+    <row r="251" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A251" s="3">
         <v>991825280</v>
       </c>
@@ -13967,7 +13976,7 @@
       <c r="U251" s="6"/>
       <c r="V251" s="6"/>
     </row>
-    <row r="252" ht="28.25">
+    <row r="252" spans="1:22" ht="29" x14ac:dyDescent="0.35">
       <c r="A252" s="3">
         <v>991827338</v>
       </c>
@@ -14015,7 +14024,7 @@
       <c r="U252" s="6"/>
       <c r="V252" s="6"/>
     </row>
-    <row r="253" ht="14.8">
+    <row r="253" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A253" s="3">
         <v>991827569</v>
       </c>
@@ -14063,7 +14072,7 @@
       <c r="U253" s="6"/>
       <c r="V253" s="6"/>
     </row>
-    <row r="254" ht="14.8">
+    <row r="254" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A254" s="3">
         <v>991829089</v>
       </c>
@@ -14111,7 +14120,7 @@
       <c r="U254" s="6"/>
       <c r="V254" s="6"/>
     </row>
-    <row r="255" ht="14.8">
+    <row r="255" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A255" s="3">
         <v>991829139</v>
       </c>
@@ -14159,7 +14168,7 @@
       <c r="U255" s="6"/>
       <c r="V255" s="6"/>
     </row>
-    <row r="256" ht="14.8">
+    <row r="256" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A256" s="3">
         <v>991829549</v>
       </c>
@@ -14207,7 +14216,7 @@
       <c r="U256" s="6"/>
       <c r="V256" s="6"/>
     </row>
-    <row r="257" ht="14.8">
+    <row r="257" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A257" s="3">
         <v>991829569</v>
       </c>
@@ -14255,7 +14264,7 @@
       <c r="U257" s="6"/>
       <c r="V257" s="6"/>
     </row>
-    <row r="258" ht="14.8">
+    <row r="258" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A258" s="3">
         <v>991829847</v>
       </c>
@@ -14303,7 +14312,7 @@
       <c r="U258" s="6"/>
       <c r="V258" s="6"/>
     </row>
-    <row r="259" ht="14.8">
+    <row r="259" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A259" s="3">
         <v>991829849</v>
       </c>
@@ -14351,7 +14360,7 @@
       <c r="U259" s="6"/>
       <c r="V259" s="6"/>
     </row>
-    <row r="260" ht="14.8">
+    <row r="260" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A260" s="3">
         <v>991829898</v>
       </c>
@@ -14391,7 +14400,7 @@
       <c r="U260" s="6"/>
       <c r="V260" s="6"/>
     </row>
-    <row r="261" ht="28.25">
+    <row r="261" spans="1:22" ht="29" x14ac:dyDescent="0.35">
       <c r="A261" s="3">
         <v>991831740</v>
       </c>
@@ -14439,7 +14448,7 @@
       <c r="U261" s="6"/>
       <c r="V261" s="6"/>
     </row>
-    <row r="262" ht="14.8">
+    <row r="262" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A262" s="3">
         <v>991834288</v>
       </c>
@@ -14487,7 +14496,7 @@
       <c r="U262" s="6"/>
       <c r="V262" s="6"/>
     </row>
-    <row r="263" ht="14.8">
+    <row r="263" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A263" s="3">
         <v>991834615</v>
       </c>
@@ -14535,7 +14544,7 @@
       <c r="U263" s="6"/>
       <c r="V263" s="6"/>
     </row>
-    <row r="264" ht="14.8">
+    <row r="264" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A264" s="3">
         <v>991835060</v>
       </c>
@@ -14583,7 +14592,7 @@
       <c r="U264" s="6"/>
       <c r="V264" s="6"/>
     </row>
-    <row r="265" ht="14.8">
+    <row r="265" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A265" s="3">
         <v>991835184</v>
       </c>
@@ -14623,7 +14632,7 @@
       <c r="U265" s="6"/>
       <c r="V265" s="6"/>
     </row>
-    <row r="266" ht="14.8">
+    <row r="266" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A266" s="3">
         <v>991835676</v>
       </c>
@@ -14673,7 +14682,7 @@
       <c r="U266" s="6"/>
       <c r="V266" s="6"/>
     </row>
-    <row r="267" ht="14.8">
+    <row r="267" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A267" s="3">
         <v>991836185</v>
       </c>
@@ -14723,7 +14732,7 @@
       <c r="U267" s="6"/>
       <c r="V267" s="6"/>
     </row>
-    <row r="268" ht="14.8">
+    <row r="268" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A268" s="3">
         <v>991837188</v>
       </c>
@@ -14771,7 +14780,7 @@
       <c r="U268" s="6"/>
       <c r="V268" s="6"/>
     </row>
-    <row r="269" ht="14.8">
+    <row r="269" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A269" s="3">
         <v>991837574</v>
       </c>
@@ -14819,7 +14828,7 @@
       <c r="U269" s="6"/>
       <c r="V269" s="6"/>
     </row>
-    <row r="270" ht="14.8">
+    <row r="270" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A270" s="3">
         <v>991838372</v>
       </c>
@@ -14871,7 +14880,7 @@
       <c r="U270" s="6"/>
       <c r="V270" s="6"/>
     </row>
-    <row r="271" ht="14.8">
+    <row r="271" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A271" s="3">
         <v>991839047</v>
       </c>
@@ -14911,7 +14920,7 @@
       <c r="U271" s="6"/>
       <c r="V271" s="6"/>
     </row>
-    <row r="272" ht="14.8">
+    <row r="272" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A272" s="3">
         <v>991839179</v>
       </c>
@@ -14951,7 +14960,7 @@
       <c r="U272" s="6"/>
       <c r="V272" s="6"/>
     </row>
-    <row r="273" ht="14.8">
+    <row r="273" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A273" s="3">
         <v>991840271</v>
       </c>
@@ -14999,7 +15008,7 @@
       <c r="U273" s="6"/>
       <c r="V273" s="6"/>
     </row>
-    <row r="274" ht="28.25">
+    <row r="274" spans="1:22" ht="29" x14ac:dyDescent="0.35">
       <c r="A274" s="3">
         <v>991840669</v>
       </c>
@@ -15047,7 +15056,7 @@
       <c r="U274" s="6"/>
       <c r="V274" s="6"/>
     </row>
-    <row r="275" ht="28.25">
+    <row r="275" spans="1:22" ht="29" x14ac:dyDescent="0.35">
       <c r="A275" s="3">
         <v>991841363</v>
       </c>
@@ -15095,7 +15104,7 @@
       <c r="U275" s="6"/>
       <c r="V275" s="6"/>
     </row>
-    <row r="276" ht="28.25">
+    <row r="276" spans="1:22" ht="29" x14ac:dyDescent="0.35">
       <c r="A276" s="3">
         <v>991842115</v>
       </c>
@@ -15155,7 +15164,7 @@
       <c r="U276" s="6"/>
       <c r="V276" s="6"/>
     </row>
-    <row r="277" ht="14.8">
+    <row r="277" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A277" s="3">
         <v>991842505</v>
       </c>
@@ -15215,7 +15224,7 @@
       <c r="U277" s="6"/>
       <c r="V277" s="6"/>
     </row>
-    <row r="278" ht="14.8">
+    <row r="278" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A278" s="3">
         <v>991842589</v>
       </c>
@@ -15275,7 +15284,7 @@
       <c r="U278" s="6"/>
       <c r="V278" s="6"/>
     </row>
-    <row r="279" ht="14.8">
+    <row r="279" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A279" s="3">
         <v>991842805</v>
       </c>
@@ -15323,7 +15332,7 @@
       <c r="U279" s="6"/>
       <c r="V279" s="6"/>
     </row>
-    <row r="280" ht="14.8">
+    <row r="280" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A280" s="3">
         <v>991844286</v>
       </c>
@@ -15371,7 +15380,7 @@
       <c r="U280" s="6"/>
       <c r="V280" s="6"/>
     </row>
-    <row r="281" ht="14.8">
+    <row r="281" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A281" s="3">
         <v>991845891</v>
       </c>
@@ -15419,7 +15428,7 @@
       <c r="U281" s="6"/>
       <c r="V281" s="6"/>
     </row>
-    <row r="282" ht="14.8">
+    <row r="282" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A282" s="3">
         <v>991846481</v>
       </c>
@@ -15467,7 +15476,7 @@
       <c r="U282" s="6"/>
       <c r="V282" s="6"/>
     </row>
-    <row r="283" ht="14.8">
+    <row r="283" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A283" s="3">
         <v>991849721</v>
       </c>
@@ -15515,7 +15524,7 @@
       <c r="U283" s="6"/>
       <c r="V283" s="6"/>
     </row>
-    <row r="284" ht="14.8">
+    <row r="284" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A284" s="3">
         <v>991872342</v>
       </c>
@@ -15561,7 +15570,7 @@
       <c r="U284" s="6"/>
       <c r="V284" s="6"/>
     </row>
-    <row r="285" ht="14.8">
+    <row r="285" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A285" s="3">
         <v>991872468</v>
       </c>
@@ -15609,7 +15618,7 @@
       <c r="U285" s="6"/>
       <c r="V285" s="6"/>
     </row>
-    <row r="286" ht="14.8">
+    <row r="286" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A286" s="3">
         <v>991872505</v>
       </c>
@@ -15657,7 +15666,7 @@
       <c r="U286" s="6"/>
       <c r="V286" s="6"/>
     </row>
-    <row r="287" ht="28.25">
+    <row r="287" spans="1:22" ht="29" x14ac:dyDescent="0.35">
       <c r="A287" s="3">
         <v>991872560</v>
       </c>
@@ -15705,7 +15714,7 @@
       <c r="U287" s="6"/>
       <c r="V287" s="6"/>
     </row>
-    <row r="288" ht="14.8">
+    <row r="288" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A288" s="3">
         <v>991872563</v>
       </c>
@@ -15751,7 +15760,7 @@
       <c r="U288" s="6"/>
       <c r="V288" s="6"/>
     </row>
-    <row r="289" ht="14.8">
+    <row r="289" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A289" s="3">
         <v>991876311</v>
       </c>
@@ -15789,7 +15798,7 @@
       <c r="U289" s="6"/>
       <c r="V289" s="6"/>
     </row>
-    <row r="290" ht="14.8">
+    <row r="290" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A290" s="3">
         <v>991876642</v>
       </c>
@@ -15833,7 +15842,7 @@
       <c r="U290" s="6"/>
       <c r="V290" s="6"/>
     </row>
-    <row r="291" ht="14.8">
+    <row r="291" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A291" s="3">
         <v>991876904</v>
       </c>
@@ -15881,7 +15890,7 @@
       <c r="U291" s="6"/>
       <c r="V291" s="6"/>
     </row>
-    <row r="292" ht="28.25">
+    <row r="292" spans="1:22" ht="29" x14ac:dyDescent="0.35">
       <c r="A292" s="3">
         <v>991877647</v>
       </c>
@@ -15929,7 +15938,7 @@
       <c r="U292" s="6"/>
       <c r="V292" s="6"/>
     </row>
-    <row r="293" ht="14.8">
+    <row r="293" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A293" s="3">
         <v>991877698</v>
       </c>
@@ -15977,7 +15986,7 @@
       <c r="U293" s="6"/>
       <c r="V293" s="6"/>
     </row>
-    <row r="294" ht="14.8">
+    <row r="294" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A294" s="3">
         <v>991879015</v>
       </c>
@@ -16025,7 +16034,7 @@
       <c r="U294" s="6"/>
       <c r="V294" s="6"/>
     </row>
-    <row r="295" ht="14.8">
+    <row r="295" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A295" s="3">
         <v>991879038</v>
       </c>
@@ -16073,7 +16082,7 @@
       <c r="U295" s="6"/>
       <c r="V295" s="6"/>
     </row>
-    <row r="296" ht="14.8">
+    <row r="296" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A296" s="3">
         <v>991879043</v>
       </c>
@@ -16121,7 +16130,7 @@
       <c r="U296" s="6"/>
       <c r="V296" s="6"/>
     </row>
-    <row r="297" ht="14.8">
+    <row r="297" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A297" s="3">
         <v>991879076</v>
       </c>
@@ -16169,7 +16178,7 @@
       <c r="U297" s="6"/>
       <c r="V297" s="6"/>
     </row>
-    <row r="298" ht="14.8">
+    <row r="298" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A298" s="3">
         <v>991879114</v>
       </c>
@@ -16209,7 +16218,7 @@
       <c r="U298" s="6"/>
       <c r="V298" s="6"/>
     </row>
-    <row r="299" ht="14.8">
+    <row r="299" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A299" s="3">
         <v>991879529</v>
       </c>
@@ -16257,7 +16266,7 @@
       <c r="U299" s="6"/>
       <c r="V299" s="6"/>
     </row>
-    <row r="300" ht="28.25">
+    <row r="300" spans="1:22" ht="29" x14ac:dyDescent="0.35">
       <c r="A300" s="3">
         <v>991881758</v>
       </c>
@@ -16305,7 +16314,7 @@
       <c r="U300" s="6"/>
       <c r="V300" s="6"/>
     </row>
-    <row r="301" ht="14.8">
+    <row r="301" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A301" s="3">
         <v>991882110</v>
       </c>
@@ -16353,7 +16362,7 @@
       <c r="U301" s="6"/>
       <c r="V301" s="6"/>
     </row>
-    <row r="302" ht="14.8">
+    <row r="302" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A302" s="3">
         <v>991882114</v>
       </c>
@@ -16401,7 +16410,7 @@
       <c r="U302" s="6"/>
       <c r="V302" s="6"/>
     </row>
-    <row r="303" ht="14.8">
+    <row r="303" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A303" s="3">
         <v>991883502</v>
       </c>
@@ -16449,7 +16458,7 @@
       <c r="U303" s="6"/>
       <c r="V303" s="6"/>
     </row>
-    <row r="304" ht="14.8">
+    <row r="304" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A304" s="3">
         <v>991886489</v>
       </c>
@@ -16497,7 +16506,7 @@
       <c r="U304" s="6"/>
       <c r="V304" s="6"/>
     </row>
-    <row r="305" ht="14.8">
+    <row r="305" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A305" s="3">
         <v>991887135</v>
       </c>
@@ -16545,7 +16554,7 @@
       <c r="U305" s="6"/>
       <c r="V305" s="6"/>
     </row>
-    <row r="306" ht="28.25">
+    <row r="306" spans="1:22" ht="29" x14ac:dyDescent="0.35">
       <c r="A306" s="3">
         <v>991900409</v>
       </c>
@@ -16593,7 +16602,7 @@
       <c r="U306" s="6"/>
       <c r="V306" s="6"/>
     </row>
-    <row r="307" ht="14.8">
+    <row r="307" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A307" s="3">
         <v>991900718</v>
       </c>
@@ -16641,7 +16650,7 @@
       <c r="U307" s="6"/>
       <c r="V307" s="6"/>
     </row>
-    <row r="308" ht="14.8">
+    <row r="308" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A308" s="3">
         <v>991901268</v>
       </c>
@@ -16689,7 +16698,7 @@
       <c r="U308" s="6"/>
       <c r="V308" s="6"/>
     </row>
-    <row r="309" ht="14.8">
+    <row r="309" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A309" s="3">
         <v>991901324</v>
       </c>
@@ -16729,7 +16738,7 @@
       <c r="U309" s="6"/>
       <c r="V309" s="6"/>
     </row>
-    <row r="310" ht="14.8">
+    <row r="310" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A310" s="3">
         <v>991901691</v>
       </c>
@@ -16777,7 +16786,7 @@
       <c r="U310" s="6"/>
       <c r="V310" s="6"/>
     </row>
-    <row r="311" ht="14.8">
+    <row r="311" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A311" s="3">
         <v>991901791</v>
       </c>
@@ -16825,7 +16834,7 @@
       <c r="U311" s="6"/>
       <c r="V311" s="6"/>
     </row>
-    <row r="312" ht="14.8">
+    <row r="312" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A312" s="3">
         <v>991902305</v>
       </c>
@@ -16863,7 +16872,7 @@
       <c r="U312" s="6"/>
       <c r="V312" s="6"/>
     </row>
-    <row r="313" ht="14.8">
+    <row r="313" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A313" s="3">
         <v>991903375</v>
       </c>
@@ -16911,7 +16920,7 @@
       <c r="U313" s="6"/>
       <c r="V313" s="6"/>
     </row>
-    <row r="314" ht="14.8">
+    <row r="314" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A314" s="3">
         <v>991904938</v>
       </c>
@@ -16959,7 +16968,7 @@
       <c r="U314" s="6"/>
       <c r="V314" s="6"/>
     </row>
-    <row r="315" ht="14.8">
+    <row r="315" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A315" s="3">
         <v>991905333</v>
       </c>
@@ -17005,7 +17014,7 @@
       <c r="U315" s="6"/>
       <c r="V315" s="6"/>
     </row>
-    <row r="316" ht="14.8">
+    <row r="316" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A316" s="3">
         <v>991905358</v>
       </c>
@@ -17051,7 +17060,7 @@
       <c r="U316" s="6"/>
       <c r="V316" s="6"/>
     </row>
-    <row r="317" ht="14.8">
+    <row r="317" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A317" s="3">
         <v>991905384</v>
       </c>
@@ -17097,7 +17106,7 @@
       <c r="U317" s="6"/>
       <c r="V317" s="6"/>
     </row>
-    <row r="318" ht="14.8">
+    <row r="318" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A318" s="3">
         <v>991907123</v>
       </c>
@@ -17145,7 +17154,7 @@
       <c r="U318" s="6"/>
       <c r="V318" s="6"/>
     </row>
-    <row r="319" ht="14.8">
+    <row r="319" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A319" s="3">
         <v>991907647</v>
       </c>
@@ -17191,7 +17200,7 @@
       <c r="U319" s="6"/>
       <c r="V319" s="6"/>
     </row>
-    <row r="320" ht="28.25">
+    <row r="320" spans="1:22" ht="29" x14ac:dyDescent="0.35">
       <c r="A320" s="3">
         <v>991908206</v>
       </c>
@@ -17239,7 +17248,7 @@
       <c r="U320" s="6"/>
       <c r="V320" s="6"/>
     </row>
-    <row r="321" ht="14.8">
+    <row r="321" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A321" s="3">
         <v>991908520</v>
       </c>
@@ -17287,7 +17296,7 @@
       <c r="U321" s="6"/>
       <c r="V321" s="6"/>
     </row>
-    <row r="322" ht="14.8">
+    <row r="322" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A322" s="3">
         <v>991909011</v>
       </c>
@@ -17327,7 +17336,7 @@
       <c r="U322" s="6"/>
       <c r="V322" s="6"/>
     </row>
-    <row r="323" ht="14.8">
+    <row r="323" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A323" s="3">
         <v>991909028</v>
       </c>
@@ -17367,7 +17376,7 @@
       <c r="U323" s="6"/>
       <c r="V323" s="6"/>
     </row>
-    <row r="324" ht="14.8">
+    <row r="324" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A324" s="3">
         <v>991910469</v>
       </c>
@@ -17415,7 +17424,7 @@
       <c r="U324" s="6"/>
       <c r="V324" s="6"/>
     </row>
-    <row r="325" ht="14.8">
+    <row r="325" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A325" s="3">
         <v>991910763</v>
       </c>
@@ -17451,7 +17460,7 @@
       <c r="U325" s="6"/>
       <c r="V325" s="6"/>
     </row>
-    <row r="326" ht="14.8">
+    <row r="326" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A326" s="3">
         <v>991910983</v>
       </c>
@@ -17499,7 +17508,7 @@
       <c r="U326" s="6"/>
       <c r="V326" s="6"/>
     </row>
-    <row r="327" ht="14.8">
+    <row r="327" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A327" s="3">
         <v>991910985</v>
       </c>
@@ -17547,7 +17556,7 @@
       <c r="U327" s="6"/>
       <c r="V327" s="6"/>
     </row>
-    <row r="328" ht="14.8">
+    <row r="328" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A328" s="3">
         <v>991911085</v>
       </c>
@@ -17587,7 +17596,7 @@
       <c r="U328" s="6"/>
       <c r="V328" s="6"/>
     </row>
-    <row r="329" ht="14.8">
+    <row r="329" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A329" s="3">
         <v>991911468</v>
       </c>
@@ -17635,7 +17644,7 @@
       <c r="U329" s="6"/>
       <c r="V329" s="6"/>
     </row>
-    <row r="330" ht="14.8">
+    <row r="330" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A330" s="3">
         <v>991911699</v>
       </c>
@@ -17675,7 +17684,7 @@
       <c r="U330" s="6"/>
       <c r="V330" s="6"/>
     </row>
-    <row r="331" ht="14.8">
+    <row r="331" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A331" s="3">
         <v>991911742</v>
       </c>
@@ -17723,7 +17732,7 @@
       <c r="U331" s="6"/>
       <c r="V331" s="6"/>
     </row>
-    <row r="332" ht="14.8">
+    <row r="332" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A332" s="3">
         <v>991912348</v>
       </c>
@@ -17771,7 +17780,7 @@
       <c r="U332" s="6"/>
       <c r="V332" s="6"/>
     </row>
-    <row r="333" ht="14.8">
+    <row r="333" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A333" s="3">
         <v>991912928</v>
       </c>
@@ -17819,7 +17828,7 @@
       <c r="U333" s="6"/>
       <c r="V333" s="6"/>
     </row>
-    <row r="334" ht="14.8">
+    <row r="334" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A334" s="3">
         <v>991912933</v>
       </c>
@@ -17867,7 +17876,7 @@
       <c r="U334" s="6"/>
       <c r="V334" s="6"/>
     </row>
-    <row r="335" ht="14.8">
+    <row r="335" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A335" s="3">
         <v>991912937</v>
       </c>
@@ -17907,7 +17916,7 @@
       <c r="U335" s="6"/>
       <c r="V335" s="6"/>
     </row>
-    <row r="336" ht="14.8">
+    <row r="336" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A336" s="3">
         <v>991915402</v>
       </c>
@@ -17947,7 +17956,7 @@
       <c r="U336" s="6"/>
       <c r="V336" s="6"/>
     </row>
-    <row r="337" ht="14.8">
+    <row r="337" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A337" s="3">
         <v>991915575</v>
       </c>
@@ -17997,7 +18006,7 @@
       <c r="U337" s="6"/>
       <c r="V337" s="6"/>
     </row>
-    <row r="338" ht="28.25">
+    <row r="338" spans="1:22" ht="29" x14ac:dyDescent="0.35">
       <c r="A338" s="3">
         <v>991915987</v>
       </c>
@@ -18045,7 +18054,7 @@
       <c r="U338" s="6"/>
       <c r="V338" s="6"/>
     </row>
-    <row r="339" ht="14.8">
+    <row r="339" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A339" s="3">
         <v>991916980</v>
       </c>
@@ -18085,7 +18094,7 @@
       <c r="U339" s="6"/>
       <c r="V339" s="6"/>
     </row>
-    <row r="340" ht="28.25">
+    <row r="340" spans="1:22" ht="29" x14ac:dyDescent="0.35">
       <c r="A340" s="3">
         <v>991918483</v>
       </c>
@@ -18133,7 +18142,7 @@
       <c r="U340" s="6"/>
       <c r="V340" s="6"/>
     </row>
-    <row r="341" ht="28.25">
+    <row r="341" spans="1:22" ht="29" x14ac:dyDescent="0.35">
       <c r="A341" s="3">
         <v>991918502</v>
       </c>
@@ -18181,7 +18190,7 @@
       <c r="U341" s="6"/>
       <c r="V341" s="6"/>
     </row>
-    <row r="342" ht="14.8">
+    <row r="342" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A342" s="3">
         <v>991919604</v>
       </c>
@@ -18229,7 +18238,7 @@
       <c r="U342" s="6"/>
       <c r="V342" s="6"/>
     </row>
-    <row r="343" ht="14.8">
+    <row r="343" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A343" s="3">
         <v>991919675</v>
       </c>
@@ -18277,7 +18286,7 @@
       <c r="U343" s="6"/>
       <c r="V343" s="6"/>
     </row>
-    <row r="344" ht="28.25">
+    <row r="344" spans="1:22" ht="29" x14ac:dyDescent="0.35">
       <c r="A344" s="3">
         <v>992068522</v>
       </c>
@@ -18325,7 +18334,7 @@
       <c r="U344" s="6"/>
       <c r="V344" s="6"/>
     </row>
-    <row r="345" ht="14.8">
+    <row r="345" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A345" s="3">
         <v>992068523</v>
       </c>
@@ -18385,7 +18394,7 @@
       <c r="U345" s="6"/>
       <c r="V345" s="6"/>
     </row>
-    <row r="346" ht="14.8">
+    <row r="346" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A346" s="3">
         <v>992069249</v>
       </c>
@@ -18425,7 +18434,7 @@
       <c r="U346" s="6"/>
       <c r="V346" s="6"/>
     </row>
-    <row r="347" ht="14.8">
+    <row r="347" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A347" s="3">
         <v>992069261</v>
       </c>
@@ -18473,7 +18482,7 @@
       <c r="U347" s="6"/>
       <c r="V347" s="6"/>
     </row>
-    <row r="348" ht="14.8">
+    <row r="348" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A348" s="3">
         <v>992069650</v>
       </c>
@@ -18533,7 +18542,7 @@
       <c r="U348" s="6"/>
       <c r="V348" s="6"/>
     </row>
-    <row r="349" ht="14.8">
+    <row r="349" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A349" s="3">
         <v>992069651</v>
       </c>
@@ -18593,7 +18602,7 @@
       <c r="U349" s="6"/>
       <c r="V349" s="6"/>
     </row>
-    <row r="350" ht="14.8">
+    <row r="350" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A350" s="3">
         <v>992071198</v>
       </c>
@@ -18641,7 +18650,7 @@
       <c r="U350" s="6"/>
       <c r="V350" s="6"/>
     </row>
-    <row r="351" ht="14.8">
+    <row r="351" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A351" s="3">
         <v>992072058</v>
       </c>
@@ -18689,7 +18698,7 @@
       <c r="U351" s="6"/>
       <c r="V351" s="6"/>
     </row>
-    <row r="352" ht="14.8">
+    <row r="352" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A352" s="3">
         <v>992073918</v>
       </c>
@@ -18737,7 +18746,7 @@
       <c r="U352" s="6"/>
       <c r="V352" s="6"/>
     </row>
-    <row r="353" ht="14.8">
+    <row r="353" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A353" s="3">
         <v>992074607</v>
       </c>
@@ -18777,7 +18786,7 @@
       <c r="U353" s="6"/>
       <c r="V353" s="6"/>
     </row>
-    <row r="354" ht="14.8">
+    <row r="354" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A354" s="3">
         <v>992075034</v>
       </c>
@@ -18825,7 +18834,7 @@
       <c r="U354" s="6"/>
       <c r="V354" s="6"/>
     </row>
-    <row r="355" ht="14.8">
+    <row r="355" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A355" s="3">
         <v>992075583</v>
       </c>
@@ -18875,7 +18884,7 @@
       <c r="U355" s="6"/>
       <c r="V355" s="6"/>
     </row>
-    <row r="356" ht="14.8">
+    <row r="356" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A356" s="3">
         <v>992075584</v>
       </c>
@@ -18923,7 +18932,7 @@
       <c r="U356" s="6"/>
       <c r="V356" s="6"/>
     </row>
-    <row r="357" ht="14.8">
+    <row r="357" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A357" s="3">
         <v>992075763</v>
       </c>
@@ -18971,7 +18980,7 @@
       <c r="U357" s="6"/>
       <c r="V357" s="6"/>
     </row>
-    <row r="358" ht="14.8">
+    <row r="358" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A358" s="3">
         <v>992075764</v>
       </c>
@@ -19019,7 +19028,7 @@
       <c r="U358" s="6"/>
       <c r="V358" s="6"/>
     </row>
-    <row r="359" ht="14.8">
+    <row r="359" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A359" s="3">
         <v>992128778</v>
       </c>
@@ -19067,7 +19076,7 @@
       <c r="U359" s="6"/>
       <c r="V359" s="6"/>
     </row>
-    <row r="360" ht="14.8">
+    <row r="360" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A360" s="3">
         <v>992129413</v>
       </c>
@@ -19127,7 +19136,7 @@
       <c r="U360" s="6"/>
       <c r="V360" s="6"/>
     </row>
-    <row r="361" ht="14.8">
+    <row r="361" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A361" s="3">
         <v>992130814</v>
       </c>
@@ -19175,7 +19184,7 @@
       <c r="U361" s="6"/>
       <c r="V361" s="6"/>
     </row>
-    <row r="362" ht="14.8">
+    <row r="362" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A362" s="3">
         <v>992131806</v>
       </c>
@@ -19215,7 +19224,7 @@
       <c r="U362" s="6"/>
       <c r="V362" s="6"/>
     </row>
-    <row r="363" ht="14.8">
+    <row r="363" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A363" s="3">
         <v>992136059</v>
       </c>
@@ -19255,7 +19264,7 @@
       <c r="U363" s="6"/>
       <c r="V363" s="6"/>
     </row>
-    <row r="364" ht="14.8">
+    <row r="364" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A364" s="3">
         <v>992137385</v>
       </c>
@@ -19307,7 +19316,7 @@
       <c r="U364" s="6"/>
       <c r="V364" s="6"/>
     </row>
-    <row r="365" ht="14.8">
+    <row r="365" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A365" s="3">
         <v>992138079</v>
       </c>
@@ -19355,7 +19364,7 @@
       <c r="U365" s="6"/>
       <c r="V365" s="6"/>
     </row>
-    <row r="366" ht="14.8">
+    <row r="366" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A366" s="3">
         <v>992138925</v>
       </c>
@@ -19395,7 +19404,7 @@
       <c r="U366" s="6"/>
       <c r="V366" s="6"/>
     </row>
-    <row r="367" ht="14.8">
+    <row r="367" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A367" s="3">
         <v>992141162</v>
       </c>
@@ -19443,7 +19452,7 @@
       <c r="U367" s="6"/>
       <c r="V367" s="6"/>
     </row>
-    <row r="368" ht="14.8">
+    <row r="368" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A368" s="3">
         <v>992141552</v>
       </c>
@@ -19491,7 +19500,7 @@
       <c r="U368" s="6"/>
       <c r="V368" s="6"/>
     </row>
-    <row r="369" ht="14.8">
+    <row r="369" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A369" s="3">
         <v>992141634</v>
       </c>
@@ -19539,7 +19548,7 @@
       <c r="U369" s="6"/>
       <c r="V369" s="6"/>
     </row>
-    <row r="370" ht="14.8">
+    <row r="370" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A370" s="3">
         <v>992141669</v>
       </c>
@@ -19579,7 +19588,7 @@
       <c r="U370" s="6"/>
       <c r="V370" s="6"/>
     </row>
-    <row r="371" ht="14.8">
+    <row r="371" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A371" s="3">
         <v>992142429</v>
       </c>
@@ -19627,7 +19636,7 @@
       <c r="U371" s="6"/>
       <c r="V371" s="6"/>
     </row>
-    <row r="372" ht="14.8">
+    <row r="372" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A372" s="3">
         <v>992144097</v>
       </c>
@@ -19675,7 +19684,7 @@
       <c r="U372" s="6"/>
       <c r="V372" s="6"/>
     </row>
-    <row r="373" ht="14.8">
+    <row r="373" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A373" s="3">
         <v>992144099</v>
       </c>
@@ -19715,7 +19724,7 @@
       <c r="U373" s="6"/>
       <c r="V373" s="6"/>
     </row>
-    <row r="374" ht="14.8">
+    <row r="374" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A374" s="3">
         <v>992144386</v>
       </c>
@@ -19763,7 +19772,7 @@
       <c r="U374" s="6"/>
       <c r="V374" s="6"/>
     </row>
-    <row r="375" ht="14.8">
+    <row r="375" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A375" s="3">
         <v>992146404</v>
       </c>
@@ -19803,7 +19812,7 @@
       <c r="U375" s="6"/>
       <c r="V375" s="6"/>
     </row>
-    <row r="376" ht="14.8">
+    <row r="376" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A376" s="3">
         <v>992146587</v>
       </c>
@@ -19843,7 +19852,7 @@
       <c r="U376" s="6"/>
       <c r="V376" s="6"/>
     </row>
-    <row r="377" ht="14.8">
+    <row r="377" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A377" s="3">
         <v>992148790</v>
       </c>
@@ -19891,7 +19900,7 @@
       <c r="U377" s="6"/>
       <c r="V377" s="6"/>
     </row>
-    <row r="378" ht="28.25">
+    <row r="378" spans="1:22" ht="29" x14ac:dyDescent="0.35">
       <c r="A378" s="3">
         <v>992150991</v>
       </c>
@@ -19939,7 +19948,7 @@
       <c r="U378" s="6"/>
       <c r="V378" s="6"/>
     </row>
-    <row r="379" ht="14.8">
+    <row r="379" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A379" s="3">
         <v>992151931</v>
       </c>
@@ -19991,7 +20000,7 @@
       <c r="U379" s="6"/>
       <c r="V379" s="6"/>
     </row>
-    <row r="380" ht="28.25">
+    <row r="380" spans="1:22" ht="29" x14ac:dyDescent="0.35">
       <c r="A380" s="3">
         <v>992154226</v>
       </c>
@@ -20039,7 +20048,7 @@
       <c r="U380" s="6"/>
       <c r="V380" s="6"/>
     </row>
-    <row r="381" ht="14.8">
+    <row r="381" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A381" s="3">
         <v>992155674</v>
       </c>
@@ -20087,7 +20096,7 @@
       <c r="U381" s="6"/>
       <c r="V381" s="6"/>
     </row>
-    <row r="382" ht="28.25">
+    <row r="382" spans="1:22" ht="29" x14ac:dyDescent="0.35">
       <c r="A382" s="3">
         <v>992155675</v>
       </c>
@@ -20135,7 +20144,7 @@
       <c r="U382" s="6"/>
       <c r="V382" s="6"/>
     </row>
-    <row r="383" ht="28.25">
+    <row r="383" spans="1:22" ht="29" x14ac:dyDescent="0.35">
       <c r="A383" s="3">
         <v>992156256</v>
       </c>
@@ -20183,7 +20192,7 @@
       <c r="U383" s="6"/>
       <c r="V383" s="6"/>
     </row>
-    <row r="384" ht="14.8">
+    <row r="384" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A384" s="3">
         <v>992156565</v>
       </c>
@@ -20223,7 +20232,7 @@
       <c r="U384" s="6"/>
       <c r="V384" s="6"/>
     </row>
-    <row r="385" ht="14.8">
+    <row r="385" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A385" s="3">
         <v>992156874</v>
       </c>
@@ -20271,7 +20280,7 @@
       <c r="U385" s="6"/>
       <c r="V385" s="6"/>
     </row>
-    <row r="386" ht="14.8">
+    <row r="386" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A386" s="3">
         <v>992156878</v>
       </c>
@@ -20321,7 +20330,7 @@
       <c r="U386" s="6"/>
       <c r="V386" s="6"/>
     </row>
-    <row r="387" ht="14.8">
+    <row r="387" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A387" s="3">
         <v>992157571</v>
       </c>
@@ -20369,7 +20378,7 @@
       <c r="U387" s="6"/>
       <c r="V387" s="6"/>
     </row>
-    <row r="388" ht="14.8">
+    <row r="388" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A388" s="3">
         <v>992158273</v>
       </c>
@@ -20429,7 +20438,7 @@
       <c r="U388" s="6"/>
       <c r="V388" s="6"/>
     </row>
-    <row r="389" ht="14.8">
+    <row r="389" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A389" s="3">
         <v>992158274</v>
       </c>
@@ -20481,7 +20490,7 @@
       <c r="U389" s="6"/>
       <c r="V389" s="6"/>
     </row>
-    <row r="390" ht="14.8">
+    <row r="390" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A390" s="3">
         <v>992159433</v>
       </c>
@@ -20521,7 +20530,7 @@
       <c r="U390" s="6"/>
       <c r="V390" s="6"/>
     </row>
-    <row r="391" ht="28.25">
+    <row r="391" spans="1:22" ht="29" x14ac:dyDescent="0.35">
       <c r="A391" s="3">
         <v>992159547</v>
       </c>
@@ -20569,7 +20578,7 @@
       <c r="U391" s="6"/>
       <c r="V391" s="6"/>
     </row>
-    <row r="392" ht="28.25">
+    <row r="392" spans="1:22" ht="29" x14ac:dyDescent="0.35">
       <c r="A392" s="3">
         <v>992159668</v>
       </c>
@@ -20617,7 +20626,7 @@
       <c r="U392" s="6"/>
       <c r="V392" s="6"/>
     </row>
-    <row r="393" ht="14.8">
+    <row r="393" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A393" s="3">
         <v>992160564</v>
       </c>
@@ -20665,7 +20674,7 @@
       <c r="U393" s="6"/>
       <c r="V393" s="6"/>
     </row>
-    <row r="394" ht="28.25">
+    <row r="394" spans="1:22" ht="29" x14ac:dyDescent="0.35">
       <c r="A394" s="3">
         <v>992161978</v>
       </c>
@@ -20713,7 +20722,7 @@
       <c r="U394" s="6"/>
       <c r="V394" s="6"/>
     </row>
-    <row r="395" ht="14.8">
+    <row r="395" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A395" s="3">
         <v>992165274</v>
       </c>
@@ -20763,7 +20772,7 @@
       <c r="U395" s="6"/>
       <c r="V395" s="6"/>
     </row>
-    <row r="396" ht="28.25">
+    <row r="396" spans="1:22" ht="29" x14ac:dyDescent="0.35">
       <c r="A396" s="3">
         <v>992167277</v>
       </c>
@@ -20811,7 +20820,7 @@
       <c r="U396" s="6"/>
       <c r="V396" s="6"/>
     </row>
-    <row r="397" ht="14.8">
+    <row r="397" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A397" s="3">
         <v>992167666</v>
       </c>
@@ -20851,7 +20860,7 @@
       <c r="U397" s="6"/>
       <c r="V397" s="6"/>
     </row>
-    <row r="398" ht="14.8">
+    <row r="398" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A398" s="3">
         <v>992168063</v>
       </c>
@@ -20891,7 +20900,7 @@
       <c r="U398" s="6"/>
       <c r="V398" s="6"/>
     </row>
-    <row r="399" ht="14.8">
+    <row r="399" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A399" s="3">
         <v>992168173</v>
       </c>
@@ -20939,7 +20948,7 @@
       <c r="U399" s="6"/>
       <c r="V399" s="6"/>
     </row>
-    <row r="400" ht="14.8">
+    <row r="400" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A400" s="3">
         <v>992168174</v>
       </c>
@@ -20987,7 +20996,7 @@
       <c r="U400" s="6"/>
       <c r="V400" s="6"/>
     </row>
-    <row r="401" ht="14.8">
+    <row r="401" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A401" s="3">
         <v>992168694</v>
       </c>
@@ -21047,7 +21056,7 @@
       <c r="U401" s="6"/>
       <c r="V401" s="6"/>
     </row>
-    <row r="402" ht="14.8">
+    <row r="402" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A402" s="3">
         <v>992168695</v>
       </c>
@@ -21107,7 +21116,7 @@
       <c r="U402" s="6"/>
       <c r="V402" s="6"/>
     </row>
-    <row r="403" ht="14.8">
+    <row r="403" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A403" s="3">
         <v>992169345</v>
       </c>
@@ -21155,7 +21164,7 @@
       <c r="U403" s="6"/>
       <c r="V403" s="6"/>
     </row>
-    <row r="404" ht="14.8">
+    <row r="404" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A404" s="3">
         <v>992169414</v>
       </c>
@@ -21207,7 +21216,7 @@
       <c r="U404" s="6"/>
       <c r="V404" s="6"/>
     </row>
-    <row r="405" ht="28.25">
+    <row r="405" spans="1:22" ht="29" x14ac:dyDescent="0.35">
       <c r="A405" s="3">
         <v>992171833</v>
       </c>
@@ -21255,7 +21264,7 @@
       <c r="U405" s="6"/>
       <c r="V405" s="6"/>
     </row>
-    <row r="406" ht="14.8">
+    <row r="406" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A406" s="3">
         <v>992172466</v>
       </c>
@@ -21303,7 +21312,7 @@
       <c r="U406" s="6"/>
       <c r="V406" s="6"/>
     </row>
-    <row r="407" ht="28.25">
+    <row r="407" spans="1:22" ht="29" x14ac:dyDescent="0.35">
       <c r="A407" s="3">
         <v>992174765</v>
       </c>
@@ -21351,7 +21360,7 @@
       <c r="U407" s="6"/>
       <c r="V407" s="6"/>
     </row>
-    <row r="408" ht="28.25">
+    <row r="408" spans="1:22" ht="29" x14ac:dyDescent="0.35">
       <c r="A408" s="3">
         <v>992174771</v>
       </c>
@@ -21399,7 +21408,7 @@
       <c r="U408" s="6"/>
       <c r="V408" s="6"/>
     </row>
-    <row r="409" ht="14.8">
+    <row r="409" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A409" s="3">
         <v>992177624</v>
       </c>
@@ -21447,7 +21456,7 @@
       <c r="U409" s="6"/>
       <c r="V409" s="6"/>
     </row>
-    <row r="410" ht="14.8">
+    <row r="410" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A410" s="3">
         <v>992177664</v>
       </c>
@@ -21495,7 +21504,7 @@
       <c r="U410" s="6"/>
       <c r="V410" s="6"/>
     </row>
-    <row r="411" ht="14.8">
+    <row r="411" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A411" s="3">
         <v>992178747</v>
       </c>
@@ -21555,7 +21564,7 @@
       <c r="U411" s="6"/>
       <c r="V411" s="6"/>
     </row>
-    <row r="412" ht="14.8">
+    <row r="412" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A412" s="3">
         <v>992179129</v>
       </c>
@@ -21603,7 +21612,7 @@
       <c r="U412" s="6"/>
       <c r="V412" s="6"/>
     </row>
-    <row r="413" ht="14.8">
+    <row r="413" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A413" s="3">
         <v>992179928</v>
       </c>
@@ -21651,7 +21660,7 @@
       <c r="U413" s="6"/>
       <c r="V413" s="6"/>
     </row>
-    <row r="414" ht="14.8">
+    <row r="414" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A414" s="3">
         <v>992180183</v>
       </c>
@@ -21699,7 +21708,7 @@
       <c r="U414" s="6"/>
       <c r="V414" s="6"/>
     </row>
-    <row r="415" ht="14.8">
+    <row r="415" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A415" s="3">
         <v>992181137</v>
       </c>
@@ -21747,7 +21756,7 @@
       <c r="U415" s="6"/>
       <c r="V415" s="6"/>
     </row>
-    <row r="416" ht="28.25">
+    <row r="416" spans="1:22" ht="29" x14ac:dyDescent="0.35">
       <c r="A416" s="3">
         <v>992181444</v>
       </c>
@@ -21795,7 +21804,7 @@
       <c r="U416" s="6"/>
       <c r="V416" s="6"/>
     </row>
-    <row r="417" ht="14.8">
+    <row r="417" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A417" s="3">
         <v>992185529</v>
       </c>
@@ -21835,7 +21844,7 @@
       <c r="U417" s="6"/>
       <c r="V417" s="6"/>
     </row>
-    <row r="418" ht="14.8">
+    <row r="418" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A418" s="3">
         <v>992188273</v>
       </c>
@@ -21883,7 +21892,7 @@
       <c r="U418" s="6"/>
       <c r="V418" s="6"/>
     </row>
-    <row r="419" ht="14.8">
+    <row r="419" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A419" s="3">
         <v>992189234</v>
       </c>
@@ -21941,7 +21950,7 @@
       <c r="U419" s="6"/>
       <c r="V419" s="6"/>
     </row>
-    <row r="420" ht="14.8">
+    <row r="420" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A420" s="3">
         <v>992192039</v>
       </c>
@@ -21989,7 +21998,7 @@
       <c r="U420" s="6"/>
       <c r="V420" s="6"/>
     </row>
-    <row r="421" ht="14.8">
+    <row r="421" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A421" s="3">
         <v>992193006</v>
       </c>
@@ -22037,7 +22046,7 @@
       <c r="U421" s="6"/>
       <c r="V421" s="6"/>
     </row>
-    <row r="422" ht="14.8">
+    <row r="422" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A422" s="3">
         <v>992194359</v>
       </c>
@@ -22085,7 +22094,7 @@
       <c r="U422" s="6"/>
       <c r="V422" s="6"/>
     </row>
-    <row r="423" ht="14.8">
+    <row r="423" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A423" s="3">
         <v>992196074</v>
       </c>
@@ -22133,7 +22142,7 @@
       <c r="U423" s="6"/>
       <c r="V423" s="6"/>
     </row>
-    <row r="424" ht="14.8">
+    <row r="424" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A424" s="3">
         <v>992196683</v>
       </c>
@@ -22181,7 +22190,7 @@
       <c r="U424" s="6"/>
       <c r="V424" s="6"/>
     </row>
-    <row r="425" ht="14.8">
+    <row r="425" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A425" s="3">
         <v>992200525</v>
       </c>
@@ -22229,7 +22238,7 @@
       <c r="U425" s="6"/>
       <c r="V425" s="6"/>
     </row>
-    <row r="426" ht="14.8">
+    <row r="426" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A426" s="3">
         <v>992200688</v>
       </c>
@@ -22267,7 +22276,7 @@
       <c r="U426" s="6"/>
       <c r="V426" s="6"/>
     </row>
-    <row r="427" ht="14.8">
+    <row r="427" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A427" s="3">
         <v>992201220</v>
       </c>
@@ -22315,7 +22324,7 @@
       <c r="U427" s="6"/>
       <c r="V427" s="6"/>
     </row>
-    <row r="428" ht="14.8">
+    <row r="428" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A428" s="3">
         <v>992201550</v>
       </c>
@@ -22363,7 +22372,7 @@
       <c r="U428" s="6"/>
       <c r="V428" s="6"/>
     </row>
-    <row r="429" ht="14.8">
+    <row r="429" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A429" s="3">
         <v>992202773</v>
       </c>
@@ -22411,7 +22420,7 @@
       <c r="U429" s="6"/>
       <c r="V429" s="6"/>
     </row>
-    <row r="430" ht="14.8">
+    <row r="430" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A430" s="3">
         <v>992203270</v>
       </c>
@@ -22459,7 +22468,7 @@
       <c r="U430" s="6"/>
       <c r="V430" s="6"/>
     </row>
-    <row r="431" ht="14.8">
+    <row r="431" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A431" s="3">
         <v>992203363</v>
       </c>
@@ -22499,7 +22508,7 @@
       <c r="U431" s="6"/>
       <c r="V431" s="6"/>
     </row>
-    <row r="432" ht="14.8">
+    <row r="432" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A432" s="3">
         <v>992205794</v>
       </c>
@@ -22547,7 +22556,7 @@
       <c r="U432" s="6"/>
       <c r="V432" s="6"/>
     </row>
-    <row r="433" ht="14.8">
+    <row r="433" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A433" s="3">
         <v>992209645</v>
       </c>
@@ -22595,7 +22604,7 @@
       <c r="U433" s="6"/>
       <c r="V433" s="6"/>
     </row>
-    <row r="434" ht="14.8">
+    <row r="434" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A434" s="3">
         <v>992209655</v>
       </c>
@@ -22635,7 +22644,7 @@
       <c r="U434" s="6"/>
       <c r="V434" s="6"/>
     </row>
-    <row r="435" ht="14.8">
+    <row r="435" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A435" s="3">
         <v>992209928</v>
       </c>
@@ -22675,7 +22684,7 @@
       <c r="U435" s="6"/>
       <c r="V435" s="6"/>
     </row>
-    <row r="436" ht="14.8">
+    <row r="436" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A436" s="3">
         <v>992210909</v>
       </c>
@@ -22715,7 +22724,7 @@
       <c r="U436" s="6"/>
       <c r="V436" s="6"/>
     </row>
-    <row r="437" ht="14.8">
+    <row r="437" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A437" s="3">
         <v>992216458</v>
       </c>
@@ -22755,7 +22764,7 @@
       <c r="U437" s="6"/>
       <c r="V437" s="6"/>
     </row>
-    <row r="438" ht="14.8">
+    <row r="438" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A438" s="3">
         <v>992217004</v>
       </c>
@@ -22803,7 +22812,7 @@
       <c r="U438" s="6"/>
       <c r="V438" s="6"/>
     </row>
-    <row r="439" ht="14.8">
+    <row r="439" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A439" s="3">
         <v>992217884</v>
       </c>
@@ -22843,7 +22852,7 @@
       <c r="U439" s="6"/>
       <c r="V439" s="6"/>
     </row>
-    <row r="440" ht="28.25">
+    <row r="440" spans="1:22" ht="29" x14ac:dyDescent="0.35">
       <c r="A440" s="3">
         <v>992218246</v>
       </c>
@@ -22891,7 +22900,7 @@
       <c r="U440" s="6"/>
       <c r="V440" s="6"/>
     </row>
-    <row r="441" ht="14.8">
+    <row r="441" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A441" s="3">
         <v>992221058</v>
       </c>
@@ -22939,7 +22948,7 @@
       <c r="U441" s="6"/>
       <c r="V441" s="6"/>
     </row>
-    <row r="442" ht="14.8">
+    <row r="442" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A442" s="3">
         <v>992221328</v>
       </c>
@@ -22987,7 +22996,7 @@
       <c r="U442" s="6"/>
       <c r="V442" s="6"/>
     </row>
-    <row r="443" ht="14.8">
+    <row r="443" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A443" s="3">
         <v>992225817</v>
       </c>
@@ -23035,7 +23044,7 @@
       <c r="U443" s="6"/>
       <c r="V443" s="6"/>
     </row>
-    <row r="444" ht="14.8">
+    <row r="444" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A444" s="3">
         <v>992225935</v>
       </c>
@@ -23083,7 +23092,7 @@
       <c r="U444" s="6"/>
       <c r="V444" s="6"/>
     </row>
-    <row r="445" ht="14.8">
+    <row r="445" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A445" s="3">
         <v>992226071</v>
       </c>
@@ -23131,7 +23140,7 @@
       <c r="U445" s="6"/>
       <c r="V445" s="6"/>
     </row>
-    <row r="446" ht="14.8">
+    <row r="446" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A446" s="3">
         <v>992226532</v>
       </c>
@@ -23171,7 +23180,7 @@
       <c r="U446" s="6"/>
       <c r="V446" s="6"/>
     </row>
-    <row r="447" ht="14.8">
+    <row r="447" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A447" s="3">
         <v>992228492</v>
       </c>
@@ -23223,7 +23232,7 @@
       <c r="U447" s="6"/>
       <c r="V447" s="6"/>
     </row>
-    <row r="448" ht="14.8">
+    <row r="448" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A448" s="3">
         <v>992230455</v>
       </c>
@@ -23263,7 +23272,7 @@
       <c r="U448" s="6"/>
       <c r="V448" s="6"/>
     </row>
-    <row r="449" ht="14.8">
+    <row r="449" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A449" s="3">
         <v>992230883</v>
       </c>
@@ -23311,7 +23320,7 @@
       <c r="U449" s="6"/>
       <c r="V449" s="6"/>
     </row>
-    <row r="450" ht="14.8">
+    <row r="450" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A450" s="3">
         <v>992231040</v>
       </c>
@@ -23359,7 +23368,7 @@
       <c r="U450" s="6"/>
       <c r="V450" s="6"/>
     </row>
-    <row r="451" ht="14.8">
+    <row r="451" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A451" s="3">
         <v>992232107</v>
       </c>
@@ -23407,7 +23416,7 @@
       <c r="U451" s="6"/>
       <c r="V451" s="6"/>
     </row>
-    <row r="452" ht="14.8">
+    <row r="452" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A452" s="3">
         <v>992232364</v>
       </c>
@@ -23455,7 +23464,7 @@
       <c r="U452" s="6"/>
       <c r="V452" s="6"/>
     </row>
-    <row r="453" ht="14.8">
+    <row r="453" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A453" s="3">
         <v>992237257</v>
       </c>
@@ -23515,7 +23524,7 @@
       <c r="U453" s="6"/>
       <c r="V453" s="6"/>
     </row>
-    <row r="454" ht="28.25">
+    <row r="454" spans="1:22" ht="29" x14ac:dyDescent="0.35">
       <c r="A454" s="3">
         <v>992237620</v>
       </c>
@@ -23563,7 +23572,7 @@
       <c r="U454" s="6"/>
       <c r="V454" s="6"/>
     </row>
-    <row r="455" ht="14.8">
+    <row r="455" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A455" s="3">
         <v>992239005</v>
       </c>
@@ -23603,7 +23612,7 @@
       <c r="U455" s="6"/>
       <c r="V455" s="6"/>
     </row>
-    <row r="456" ht="28.25">
+    <row r="456" spans="1:22" ht="29" x14ac:dyDescent="0.35">
       <c r="A456" s="3">
         <v>992240137</v>
       </c>
@@ -23651,7 +23660,7 @@
       <c r="U456" s="6"/>
       <c r="V456" s="6"/>
     </row>
-    <row r="457" ht="14.8">
+    <row r="457" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A457" s="3">
         <v>992240969</v>
       </c>
@@ -23699,7 +23708,7 @@
       <c r="U457" s="6"/>
       <c r="V457" s="6"/>
     </row>
-    <row r="458" ht="28.25">
+    <row r="458" spans="1:22" ht="29" x14ac:dyDescent="0.35">
       <c r="A458" s="3">
         <v>992241021</v>
       </c>
@@ -23747,7 +23756,7 @@
       <c r="U458" s="6"/>
       <c r="V458" s="6"/>
     </row>
-    <row r="459" ht="14.8">
+    <row r="459" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A459" s="3">
         <v>992241570</v>
       </c>
@@ -23795,7 +23804,7 @@
       <c r="U459" s="6"/>
       <c r="V459" s="6"/>
     </row>
-    <row r="460" ht="14.8">
+    <row r="460" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A460" s="3">
         <v>992241572</v>
       </c>
@@ -23843,7 +23852,7 @@
       <c r="U460" s="6"/>
       <c r="V460" s="6"/>
     </row>
-    <row r="461" ht="14.8">
+    <row r="461" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A461" s="3">
         <v>992242743</v>
       </c>
@@ -23891,7 +23900,7 @@
       <c r="U461" s="6"/>
       <c r="V461" s="6"/>
     </row>
-    <row r="462" ht="14.8">
+    <row r="462" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A462" s="3">
         <v>992243410</v>
       </c>
@@ -23931,7 +23940,7 @@
       <c r="U462" s="6"/>
       <c r="V462" s="6"/>
     </row>
-    <row r="463" ht="14.8">
+    <row r="463" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A463" s="3">
         <v>992243587</v>
       </c>
@@ -23979,7 +23988,7 @@
       <c r="U463" s="6"/>
       <c r="V463" s="6"/>
     </row>
-    <row r="464" ht="14.8">
+    <row r="464" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A464" s="3">
         <v>992243593</v>
       </c>
@@ -24027,7 +24036,7 @@
       <c r="U464" s="6"/>
       <c r="V464" s="6"/>
     </row>
-    <row r="465" ht="14.8">
+    <row r="465" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A465" s="3">
         <v>992251000</v>
       </c>
@@ -24075,7 +24084,7 @@
       <c r="U465" s="6"/>
       <c r="V465" s="6"/>
     </row>
-    <row r="466" ht="14.8">
+    <row r="466" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A466" s="3">
         <v>992256654</v>
       </c>
@@ -24115,7 +24124,7 @@
       <c r="U466" s="6"/>
       <c r="V466" s="6"/>
     </row>
-    <row r="467" ht="14.8">
+    <row r="467" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A467" s="3">
         <v>992257617</v>
       </c>
@@ -24163,7 +24172,7 @@
       <c r="U467" s="6"/>
       <c r="V467" s="6"/>
     </row>
-    <row r="468" ht="14.8">
+    <row r="468" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A468" s="3">
         <v>992260205</v>
       </c>
@@ -24215,7 +24224,7 @@
       <c r="U468" s="6"/>
       <c r="V468" s="6"/>
     </row>
-    <row r="469" ht="14.8">
+    <row r="469" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A469" s="3">
         <v>992260669</v>
       </c>
@@ -24275,7 +24284,7 @@
       <c r="U469" s="6"/>
       <c r="V469" s="6"/>
     </row>
-    <row r="470" ht="14.8">
+    <row r="470" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A470" s="3">
         <v>992261502</v>
       </c>
@@ -24313,7 +24322,7 @@
       <c r="U470" s="6"/>
       <c r="V470" s="6"/>
     </row>
-    <row r="471" ht="14.8">
+    <row r="471" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A471" s="3">
         <v>992261504</v>
       </c>
@@ -24361,7 +24370,7 @@
       <c r="U471" s="6"/>
       <c r="V471" s="6"/>
     </row>
-    <row r="472" ht="14.8">
+    <row r="472" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A472" s="3">
         <v>992262162</v>
       </c>
@@ -24413,7 +24422,7 @@
       <c r="U472" s="6"/>
       <c r="V472" s="6"/>
     </row>
-    <row r="473" ht="14.8">
+    <row r="473" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A473" s="3">
         <v>992263969</v>
       </c>
@@ -24453,7 +24462,7 @@
       <c r="U473" s="6"/>
       <c r="V473" s="6"/>
     </row>
-    <row r="474" ht="14.8">
+    <row r="474" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A474" s="3">
         <v>992265006</v>
       </c>
@@ -24493,7 +24502,7 @@
       <c r="U474" s="6"/>
       <c r="V474" s="6"/>
     </row>
-    <row r="475" ht="14.8">
+    <row r="475" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A475" s="3">
         <v>992265271</v>
       </c>
@@ -24541,7 +24550,7 @@
       <c r="U475" s="6"/>
       <c r="V475" s="6"/>
     </row>
-    <row r="476" ht="14.8">
+    <row r="476" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A476" s="3">
         <v>992265542</v>
       </c>
@@ -24589,7 +24598,7 @@
       <c r="U476" s="6"/>
       <c r="V476" s="6"/>
     </row>
-    <row r="477" ht="14.8">
+    <row r="477" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A477" s="3">
         <v>992266451</v>
       </c>
@@ -24631,7 +24640,7 @@
       <c r="U477" s="6"/>
       <c r="V477" s="6"/>
     </row>
-    <row r="478" ht="14.8">
+    <row r="478" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A478" s="3">
         <v>992267452</v>
       </c>
@@ -24679,7 +24688,7 @@
       <c r="U478" s="6"/>
       <c r="V478" s="6"/>
     </row>
-    <row r="479" ht="14.8">
+    <row r="479" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A479" s="3">
         <v>992270771</v>
       </c>
@@ -24727,7 +24736,7 @@
       <c r="U479" s="6"/>
       <c r="V479" s="6"/>
     </row>
-    <row r="480" ht="28.25">
+    <row r="480" spans="1:22" ht="29" x14ac:dyDescent="0.35">
       <c r="A480" s="3">
         <v>992271353</v>
       </c>
@@ -24775,7 +24784,7 @@
       <c r="U480" s="6"/>
       <c r="V480" s="6"/>
     </row>
-    <row r="481" ht="14.8">
+    <row r="481" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A481" s="3">
         <v>992271455</v>
       </c>
@@ -24815,7 +24824,7 @@
       <c r="U481" s="6"/>
       <c r="V481" s="6"/>
     </row>
-    <row r="482" ht="14.8">
+    <row r="482" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A482" s="3">
         <v>992271601</v>
       </c>
@@ -24855,7 +24864,7 @@
       <c r="U482" s="6"/>
       <c r="V482" s="6"/>
     </row>
-    <row r="483" ht="14.8">
+    <row r="483" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A483" s="3">
         <v>992273033</v>
       </c>
@@ -24903,7 +24912,7 @@
       <c r="U483" s="6"/>
       <c r="V483" s="6"/>
     </row>
-    <row r="484" ht="14.8">
+    <row r="484" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A484" s="3">
         <v>992275299</v>
       </c>
@@ -24951,7 +24960,7 @@
       <c r="U484" s="6"/>
       <c r="V484" s="6"/>
     </row>
-    <row r="485" ht="28.25">
+    <row r="485" spans="1:22" ht="29" x14ac:dyDescent="0.35">
       <c r="A485" s="3">
         <v>992275425</v>
       </c>
@@ -24999,7 +25008,7 @@
       <c r="U485" s="6"/>
       <c r="V485" s="6"/>
     </row>
-    <row r="486" ht="14.8">
+    <row r="486" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A486" s="3">
         <v>992275968</v>
       </c>
@@ -25047,7 +25056,7 @@
       <c r="U486" s="6"/>
       <c r="V486" s="6"/>
     </row>
-    <row r="487" ht="14.8">
+    <row r="487" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A487" s="3">
         <v>992276115</v>
       </c>
@@ -25095,7 +25104,7 @@
       <c r="U487" s="6"/>
       <c r="V487" s="6"/>
     </row>
-    <row r="488" ht="14.8">
+    <row r="488" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A488" s="3">
         <v>992276270</v>
       </c>
@@ -25155,7 +25164,7 @@
       <c r="U488" s="6"/>
       <c r="V488" s="6"/>
     </row>
-    <row r="489" ht="14.8">
+    <row r="489" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A489" s="3">
         <v>992276609</v>
       </c>
@@ -25203,7 +25212,7 @@
       <c r="U489" s="6"/>
       <c r="V489" s="6"/>
     </row>
-    <row r="490" ht="14.8">
+    <row r="490" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A490" s="3">
         <v>992276625</v>
       </c>
@@ -25263,7 +25272,7 @@
       <c r="U490" s="6"/>
       <c r="V490" s="6"/>
     </row>
-    <row r="491" ht="14.8">
+    <row r="491" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A491" s="3">
         <v>992277011</v>
       </c>
@@ -25311,7 +25320,7 @@
       <c r="U491" s="6"/>
       <c r="V491" s="6"/>
     </row>
-    <row r="492" ht="14.8">
+    <row r="492" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A492" s="3">
         <v>992277470</v>
       </c>
@@ -25371,7 +25380,7 @@
       <c r="U492" s="6"/>
       <c r="V492" s="6"/>
     </row>
-    <row r="493" ht="14.8">
+    <row r="493" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A493" s="3">
         <v>992278015</v>
       </c>
@@ -25419,7 +25428,7 @@
       <c r="U493" s="6"/>
       <c r="V493" s="6"/>
     </row>
-    <row r="494" ht="14.8">
+    <row r="494" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A494" s="3">
         <v>992278103</v>
       </c>
@@ -25467,7 +25476,7 @@
       <c r="U494" s="6"/>
       <c r="V494" s="6"/>
     </row>
-    <row r="495" ht="14.8">
+    <row r="495" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A495" s="3">
         <v>992278556</v>
       </c>
@@ -25507,7 +25516,7 @@
       <c r="U495" s="6"/>
       <c r="V495" s="6"/>
     </row>
-    <row r="496" ht="14.8">
+    <row r="496" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A496" s="3">
         <v>992280563</v>
       </c>
@@ -25547,7 +25556,7 @@
       <c r="U496" s="6"/>
       <c r="V496" s="6"/>
     </row>
-    <row r="497" ht="14.8">
+    <row r="497" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A497" s="3">
         <v>992280769</v>
       </c>
@@ -25595,7 +25604,7 @@
       <c r="U497" s="6"/>
       <c r="V497" s="6"/>
     </row>
-    <row r="498" ht="14.8">
+    <row r="498" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A498" s="3">
         <v>992280770</v>
       </c>
@@ -25643,7 +25652,7 @@
       <c r="U498" s="6"/>
       <c r="V498" s="6"/>
     </row>
-    <row r="499" ht="14.8">
+    <row r="499" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A499" s="3">
         <v>992281327</v>
       </c>
@@ -25683,7 +25692,7 @@
       <c r="U499" s="6"/>
       <c r="V499" s="6"/>
     </row>
-    <row r="500" ht="14.8">
+    <row r="500" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A500" s="3">
         <v>992281350</v>
       </c>
@@ -25723,7 +25732,7 @@
       <c r="U500" s="6"/>
       <c r="V500" s="6"/>
     </row>
-    <row r="501" ht="14.8">
+    <row r="501" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A501" s="3">
         <v>992282143</v>
       </c>
@@ -25771,7 +25780,7 @@
       <c r="U501" s="6"/>
       <c r="V501" s="6"/>
     </row>
-    <row r="502" ht="14.8">
+    <row r="502" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A502" s="3">
         <v>992282252</v>
       </c>
@@ -25819,7 +25828,7 @@
       <c r="U502" s="6"/>
       <c r="V502" s="6"/>
     </row>
-    <row r="503" ht="14.8">
+    <row r="503" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A503" s="3">
         <v>992282819</v>
       </c>
@@ -25859,7 +25868,7 @@
       <c r="U503" s="6"/>
       <c r="V503" s="6"/>
     </row>
-    <row r="504" ht="14.8">
+    <row r="504" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A504" s="3">
         <v>992282867</v>
       </c>
@@ -25919,7 +25928,7 @@
       <c r="U504" s="6"/>
       <c r="V504" s="6"/>
     </row>
-    <row r="505" ht="14.8">
+    <row r="505" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A505" s="3">
         <v>992284250</v>
       </c>
@@ -25967,7 +25976,7 @@
       <c r="U505" s="6"/>
       <c r="V505" s="6"/>
     </row>
-    <row r="506" ht="14.8">
+    <row r="506" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A506" s="3">
         <v>992285849</v>
       </c>
@@ -26015,7 +26024,7 @@
       <c r="U506" s="6"/>
       <c r="V506" s="6"/>
     </row>
-    <row r="507" ht="14.8">
+    <row r="507" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A507" s="3">
         <v>992285851</v>
       </c>
@@ -26055,7 +26064,7 @@
       <c r="U507" s="6"/>
       <c r="V507" s="6"/>
     </row>
-    <row r="508" ht="14.8">
+    <row r="508" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A508" s="3">
         <v>992287650</v>
       </c>
@@ -26105,7 +26114,7 @@
       <c r="U508" s="6"/>
       <c r="V508" s="6"/>
     </row>
-    <row r="509" ht="14.8">
+    <row r="509" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A509" s="3">
         <v>992288354</v>
       </c>
@@ -26153,7 +26162,7 @@
       <c r="U509" s="6"/>
       <c r="V509" s="6"/>
     </row>
-    <row r="510" ht="14.8">
+    <row r="510" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A510" s="3">
         <v>992288356</v>
       </c>
@@ -26201,7 +26210,7 @@
       <c r="U510" s="6"/>
       <c r="V510" s="6"/>
     </row>
-    <row r="511" ht="14.8">
+    <row r="511" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A511" s="3">
         <v>992289251</v>
       </c>
@@ -26251,7 +26260,7 @@
       <c r="U511" s="6"/>
       <c r="V511" s="6"/>
     </row>
-    <row r="512" ht="14.8">
+    <row r="512" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A512" s="3">
         <v>992289296</v>
       </c>
@@ -26301,7 +26310,7 @@
       <c r="U512" s="6"/>
       <c r="V512" s="6"/>
     </row>
-    <row r="513" ht="14.8">
+    <row r="513" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A513" s="3">
         <v>992289309</v>
       </c>
@@ -26351,7 +26360,7 @@
       <c r="U513" s="6"/>
       <c r="V513" s="6"/>
     </row>
-    <row r="514" ht="14.8">
+    <row r="514" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A514" s="3">
         <v>992290966</v>
       </c>
@@ -26399,7 +26408,7 @@
       <c r="U514" s="6"/>
       <c r="V514" s="6"/>
     </row>
-    <row r="515" ht="14.8">
+    <row r="515" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A515" s="3">
         <v>992292620</v>
       </c>
@@ -26447,7 +26456,7 @@
       <c r="U515" s="6"/>
       <c r="V515" s="6"/>
     </row>
-    <row r="516" ht="14.8">
+    <row r="516" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A516" s="3">
         <v>992293828</v>
       </c>
@@ -26495,7 +26504,7 @@
       <c r="U516" s="6"/>
       <c r="V516" s="6"/>
     </row>
-    <row r="517" ht="14.8">
+    <row r="517" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A517" s="3">
         <v>992295007</v>
       </c>
@@ -26543,7 +26552,7 @@
       <c r="U517" s="6"/>
       <c r="V517" s="6"/>
     </row>
-    <row r="518" ht="14.8">
+    <row r="518" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A518" s="3">
         <v>992296112</v>
       </c>
@@ -26591,7 +26600,7 @@
       <c r="U518" s="6"/>
       <c r="V518" s="6"/>
     </row>
-    <row r="519" ht="14.8">
+    <row r="519" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A519" s="3">
         <v>992296940</v>
       </c>
@@ -26639,7 +26648,7 @@
       <c r="U519" s="6"/>
       <c r="V519" s="6"/>
     </row>
-    <row r="520" ht="14.8">
+    <row r="520" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A520" s="3">
         <v>992298459</v>
       </c>
@@ -26687,7 +26696,7 @@
       <c r="U520" s="6"/>
       <c r="V520" s="6"/>
     </row>
-    <row r="521" ht="14.8">
+    <row r="521" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A521" s="3">
         <v>992299172</v>
       </c>
@@ -26737,7 +26746,7 @@
       <c r="U521" s="6"/>
       <c r="V521" s="6"/>
     </row>
-    <row r="522" ht="28.25">
+    <row r="522" spans="1:22" ht="29" x14ac:dyDescent="0.35">
       <c r="A522" s="3">
         <v>992299994</v>
       </c>
@@ -26785,7 +26794,7 @@
       <c r="U522" s="6"/>
       <c r="V522" s="6"/>
     </row>
-    <row r="523" ht="14.8">
+    <row r="523" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A523" s="3">
         <v>992301388</v>
       </c>
@@ -26845,7 +26854,7 @@
       <c r="U523" s="6"/>
       <c r="V523" s="6"/>
     </row>
-    <row r="524" ht="28.25">
+    <row r="524" spans="1:22" ht="29" x14ac:dyDescent="0.35">
       <c r="A524" s="3">
         <v>992302927</v>
       </c>
@@ -26905,7 +26914,7 @@
       <c r="U524" s="6"/>
       <c r="V524" s="6"/>
     </row>
-    <row r="525" ht="14.8">
+    <row r="525" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A525" s="3">
         <v>992302974</v>
       </c>
@@ -26953,7 +26962,7 @@
       <c r="U525" s="6"/>
       <c r="V525" s="6"/>
     </row>
-    <row r="526" ht="14.8">
+    <row r="526" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A526" s="3">
         <v>992303293</v>
       </c>
@@ -27001,7 +27010,7 @@
       <c r="U526" s="6"/>
       <c r="V526" s="6"/>
     </row>
-    <row r="527" ht="14.8">
+    <row r="527" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A527" s="3">
         <v>992306048</v>
       </c>
@@ -27049,7 +27058,7 @@
       <c r="U527" s="6"/>
       <c r="V527" s="6"/>
     </row>
-    <row r="528" ht="14.8">
+    <row r="528" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A528" s="3">
         <v>992306300</v>
       </c>
@@ -27097,7 +27106,7 @@
       <c r="U528" s="6"/>
       <c r="V528" s="6"/>
     </row>
-    <row r="529" ht="14.8">
+    <row r="529" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A529" s="3">
         <v>992306719</v>
       </c>
@@ -27145,7 +27154,7 @@
       <c r="U529" s="6"/>
       <c r="V529" s="6"/>
     </row>
-    <row r="530" ht="14.8">
+    <row r="530" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A530" s="3">
         <v>992307572</v>
       </c>
@@ -27193,7 +27202,7 @@
       <c r="U530" s="6"/>
       <c r="V530" s="6"/>
     </row>
-    <row r="531" ht="14.8">
+    <row r="531" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A531" s="3">
         <v>992307603</v>
       </c>
@@ -27241,7 +27250,7 @@
       <c r="U531" s="6"/>
       <c r="V531" s="6"/>
     </row>
-    <row r="532" ht="14.8">
+    <row r="532" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A532" s="3">
         <v>992308178</v>
       </c>
@@ -27289,7 +27298,7 @@
       <c r="U532" s="6"/>
       <c r="V532" s="6"/>
     </row>
-    <row r="533" ht="14.8">
+    <row r="533" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A533" s="3">
         <v>992308514</v>
       </c>
@@ -27337,7 +27346,7 @@
       <c r="U533" s="6"/>
       <c r="V533" s="6"/>
     </row>
-    <row r="534" ht="14.8">
+    <row r="534" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A534" s="3">
         <v>992309581</v>
       </c>
@@ -27385,7 +27394,7 @@
       <c r="U534" s="6"/>
       <c r="V534" s="6"/>
     </row>
-    <row r="535" ht="14.8">
+    <row r="535" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A535" s="3">
         <v>992309632</v>
       </c>
@@ -27433,7 +27442,7 @@
       <c r="U535" s="6"/>
       <c r="V535" s="6"/>
     </row>
-    <row r="536" ht="14.8">
+    <row r="536" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A536" s="3">
         <v>992311291</v>
       </c>
@@ -27481,7 +27490,7 @@
       <c r="U536" s="6"/>
       <c r="V536" s="6"/>
     </row>
-    <row r="537" ht="14.8">
+    <row r="537" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A537" s="3">
         <v>992313533</v>
       </c>
@@ -27532,9 +27541,9 @@
       <c r="V537" s="6"/>
     </row>
   </sheetData>
-  <pageMargins left="0.69999999999999996" right="0.69999999999999996" top="0.75" bottom="0.75" header="0.29999999999999999" footer="0.29999999999999999"/>
-  <pageSetup orientation="portrait" scale="100" paperSize="1" fitToWidth="0" fitToHeight="0" horizontalDpi="0" verticalDpi="0" copies="1"/>
-  <headerFooter alignWithMargins="0" scaleWithDoc="0">
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup fitToWidth="0" fitToHeight="0" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <headerFooter scaleWithDoc="0" alignWithMargins="0">
     <oddHeader>&amp;L&amp;CList of Contacts - Referrals - Inbound - 8/18/2025&amp;R</oddHeader>
     <oddFooter>&amp;L&amp;C&amp;R</oddFooter>
   </headerFooter>

</xml_diff>